<commit_message>
Change  epo:hasBeginning to time:hasBeginning and epo:hasEnd to time:hasEnd in the conceptual_mappings.xlsx for F25
</commit_message>
<xml_diff>
--- a/mappings/package_F25/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_F25/transformation/conceptual_mappings.xlsx
@@ -2783,7 +2783,7 @@
     <t xml:space="preserve">epo:Lot / epo:ContractTerm / epo:Period / xsd:datetime</t>
   </si>
   <si>
-    <t xml:space="preserve">?this epo:foreseesContractSpecificTerm / epo:definesContractPeriod / epo:hasBeginning ?value .</t>
+    <t xml:space="preserve">?this epo:foreseesContractSpecificTerm / epo:definesContractPeriod / time:hasBeginning ?value .</t>
   </si>
   <si>
     <t xml:space="preserve">II.2.7.3</t>
@@ -2801,7 +2801,7 @@
     <t xml:space="preserve">OBJECT_CONTRACT/OBJECT_DESCR/DATE_END</t>
   </si>
   <si>
-    <t xml:space="preserve">?this epo:foreseesContractSpecificTerm / epo:definesContractPeriod / epo:hasEnd ?value .</t>
+    <t xml:space="preserve">?this epo:foreseesContractSpecificTerm / epo:definesContractPeriod / time:hasEnd ?value .</t>
   </si>
   <si>
     <t xml:space="preserve">II.2.13</t>
@@ -4727,7 +4727,7 @@
     <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="168" formatCode="General"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -4827,12 +4827,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -5042,7 +5036,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="109">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5323,10 +5317,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5391,7 +5381,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5403,7 +5393,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5415,7 +5405,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5427,7 +5417,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5467,7 +5457,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5479,7 +5469,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5605,7 +5595,7 @@
       <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.38"/>
@@ -8700,14 +8690,14 @@
   <dimension ref="A1:Z236"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="J69" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="G49" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="A69" activeCellId="0" sqref="A69"/>
-      <selection pane="bottomRight" activeCell="L81" activeCellId="0" sqref="L81"/>
+      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="A49" activeCellId="0" sqref="A49"/>
+      <selection pane="bottomRight" activeCell="H64" activeCellId="0" sqref="H64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.26"/>
@@ -10600,7 +10590,7 @@
       <c r="Q58" s="19"/>
       <c r="R58" s="19"/>
     </row>
-    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="50.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="53" t="s">
         <v>318</v>
       </c>
@@ -10634,7 +10624,7 @@
       <c r="Q59" s="19"/>
       <c r="R59" s="19"/>
     </row>
-    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="50.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="53" t="s">
         <v>325</v>
       </c>
@@ -11333,7 +11323,7 @@
       </c>
       <c r="I82" s="3"/>
       <c r="J82" s="3"/>
-      <c r="K82" s="70" t="s">
+      <c r="K82" s="19" t="s">
         <v>426</v>
       </c>
       <c r="L82" s="19"/>
@@ -11402,7 +11392,7 @@
       <c r="A85" s="57" t="s">
         <v>429</v>
       </c>
-      <c r="B85" s="71"/>
+      <c r="B85" s="70"/>
       <c r="C85" s="40"/>
       <c r="D85" s="3"/>
       <c r="E85" s="40" t="s">
@@ -11467,12 +11457,12 @@
       <c r="B87" s="38" t="s">
         <v>441</v>
       </c>
-      <c r="C87" s="72"/>
-      <c r="D87" s="72"/>
-      <c r="E87" s="73" t="s">
+      <c r="C87" s="71"/>
+      <c r="D87" s="71"/>
+      <c r="E87" s="72" t="s">
         <v>397</v>
       </c>
-      <c r="F87" s="72"/>
+      <c r="F87" s="71"/>
       <c r="G87" s="10" t="s">
         <v>442</v>
       </c>
@@ -11603,7 +11593,7 @@
       <c r="B93" s="45" t="s">
         <v>469</v>
       </c>
-      <c r="C93" s="74" t="s">
+      <c r="C93" s="73" t="s">
         <v>470</v>
       </c>
       <c r="D93" s="40"/>
@@ -11658,7 +11648,7 @@
       <c r="G95" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="H95" s="75" t="s">
+      <c r="H95" s="74" t="s">
         <v>478</v>
       </c>
       <c r="I95" s="3"/>
@@ -11684,7 +11674,7 @@
       <c r="G96" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="H96" s="76" t="s">
+      <c r="H96" s="75" t="s">
         <v>481</v>
       </c>
       <c r="I96" s="3"/>
@@ -11894,7 +11884,7 @@
       <c r="G104" s="35" t="s">
         <v>497</v>
       </c>
-      <c r="H104" s="76" t="s">
+      <c r="H104" s="75" t="s">
         <v>506</v>
       </c>
       <c r="I104" s="3"/>
@@ -11946,7 +11936,7 @@
       <c r="G106" s="3" t="s">
         <v>515</v>
       </c>
-      <c r="H106" s="77" t="s">
+      <c r="H106" s="76" t="s">
         <v>516</v>
       </c>
       <c r="I106" s="3"/>
@@ -12099,7 +12089,7 @@
       <c r="B113" s="47" t="s">
         <v>211</v>
       </c>
-      <c r="C113" s="78" t="s">
+      <c r="C113" s="77" t="s">
         <v>548</v>
       </c>
       <c r="D113" s="48"/>
@@ -12143,7 +12133,7 @@
       <c r="J114" s="3"/>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="79" t="s">
+      <c r="A115" s="78" t="s">
         <v>558</v>
       </c>
       <c r="B115" s="24" t="s">
@@ -12171,14 +12161,14 @@
       <c r="D116" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="E116" s="80" t="s">
+      <c r="E116" s="79" t="s">
         <v>561</v>
       </c>
-      <c r="F116" s="80"/>
-      <c r="G116" s="81" t="s">
+      <c r="F116" s="79"/>
+      <c r="G116" s="80" t="s">
         <v>166</v>
       </c>
-      <c r="H116" s="82" t="s">
+      <c r="H116" s="81" t="s">
         <v>562</v>
       </c>
       <c r="I116" s="3"/>
@@ -12195,8 +12185,8 @@
         <v>405</v>
       </c>
       <c r="D117" s="3"/>
-      <c r="E117" s="83"/>
-      <c r="F117" s="83"/>
+      <c r="E117" s="82"/>
+      <c r="F117" s="82"/>
       <c r="G117" s="3"/>
       <c r="H117" s="3"/>
       <c r="I117" s="3"/>
@@ -12209,7 +12199,7 @@
       <c r="B118" s="38" t="s">
         <v>566</v>
       </c>
-      <c r="C118" s="84" t="s">
+      <c r="C118" s="83" t="s">
         <v>405</v>
       </c>
       <c r="D118" s="3"/>
@@ -12467,10 +12457,10 @@
       <c r="B128" s="38" t="s">
         <v>591</v>
       </c>
-      <c r="C128" s="84" t="s">
+      <c r="C128" s="83" t="s">
         <v>405</v>
       </c>
-      <c r="D128" s="85"/>
+      <c r="D128" s="84"/>
       <c r="E128" s="3" t="s">
         <v>567</v>
       </c>
@@ -12478,7 +12468,7 @@
       <c r="G128" s="10" t="s">
         <v>592</v>
       </c>
-      <c r="H128" s="86" t="s">
+      <c r="H128" s="85" t="s">
         <v>569</v>
       </c>
       <c r="I128" s="3"/>
@@ -12735,10 +12725,10 @@
         <v>615</v>
       </c>
       <c r="F138" s="10"/>
-      <c r="G138" s="81" t="s">
+      <c r="G138" s="80" t="s">
         <v>616</v>
       </c>
-      <c r="H138" s="82" t="s">
+      <c r="H138" s="81" t="s">
         <v>617</v>
       </c>
       <c r="I138" s="3"/>
@@ -13013,14 +13003,14 @@
       <c r="D149" s="40" t="s">
         <v>642</v>
       </c>
-      <c r="E149" s="87" t="s">
+      <c r="E149" s="86" t="s">
         <v>643</v>
       </c>
-      <c r="F149" s="87"/>
-      <c r="G149" s="88" t="s">
+      <c r="F149" s="86"/>
+      <c r="G149" s="87" t="s">
         <v>644</v>
       </c>
-      <c r="H149" s="88" t="s">
+      <c r="H149" s="87" t="s">
         <v>645</v>
       </c>
       <c r="I149" s="3"/>
@@ -13062,7 +13052,7 @@
       <c r="G151" s="47" t="s">
         <v>652</v>
       </c>
-      <c r="H151" s="89" t="s">
+      <c r="H151" s="88" t="s">
         <v>653</v>
       </c>
       <c r="I151" s="3"/>
@@ -13124,7 +13114,7 @@
       <c r="G154" s="47" t="s">
         <v>652</v>
       </c>
-      <c r="H154" s="89" t="s">
+      <c r="H154" s="88" t="s">
         <v>663</v>
       </c>
       <c r="I154" s="3"/>
@@ -13146,7 +13136,7 @@
       <c r="G155" s="47" t="s">
         <v>652</v>
       </c>
-      <c r="H155" s="90" t="s">
+      <c r="H155" s="89" t="s">
         <v>667</v>
       </c>
       <c r="I155" s="3"/>
@@ -13166,12 +13156,12 @@
       <c r="G156" s="47" t="s">
         <v>652</v>
       </c>
-      <c r="H156" s="90" t="s">
+      <c r="H156" s="89" t="s">
         <v>670</v>
       </c>
       <c r="I156" s="3"/>
       <c r="J156" s="3"/>
-      <c r="K156" s="91" t="s">
+      <c r="K156" s="90" t="s">
         <v>671</v>
       </c>
     </row>
@@ -13200,7 +13190,7 @@
       <c r="B158" s="47" t="s">
         <v>675</v>
       </c>
-      <c r="C158" s="92" t="s">
+      <c r="C158" s="91" t="s">
         <v>423</v>
       </c>
       <c r="D158" s="48"/>
@@ -13211,7 +13201,7 @@
       <c r="G158" s="47" t="s">
         <v>652</v>
       </c>
-      <c r="H158" s="89" t="s">
+      <c r="H158" s="88" t="s">
         <v>677</v>
       </c>
       <c r="I158" s="3"/>
@@ -13248,7 +13238,7 @@
       <c r="D160" s="48" t="s">
         <v>683</v>
       </c>
-      <c r="E160" s="93" t="s">
+      <c r="E160" s="92" t="s">
         <v>684</v>
       </c>
       <c r="F160" s="48"/>
@@ -13262,382 +13252,382 @@
       <c r="J160" s="3"/>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="94"/>
+      <c r="A161" s="93"/>
       <c r="G161" s="19"/>
       <c r="H161" s="19"/>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="94"/>
+      <c r="A162" s="93"/>
       <c r="G162" s="19"/>
       <c r="H162" s="19"/>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="94"/>
+      <c r="A163" s="93"/>
       <c r="G163" s="19"/>
       <c r="H163" s="19"/>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="94"/>
+      <c r="A164" s="93"/>
       <c r="G164" s="19"/>
       <c r="H164" s="19"/>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="94"/>
+      <c r="A165" s="93"/>
       <c r="G165" s="19"/>
       <c r="H165" s="19"/>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="94"/>
+      <c r="A166" s="93"/>
       <c r="G166" s="19"/>
       <c r="H166" s="19"/>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="94"/>
+      <c r="A167" s="93"/>
       <c r="G167" s="19"/>
       <c r="H167" s="19"/>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="94"/>
+      <c r="A168" s="93"/>
       <c r="G168" s="19"/>
       <c r="H168" s="19"/>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="94"/>
+      <c r="A169" s="93"/>
       <c r="G169" s="19"/>
       <c r="H169" s="19"/>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="94"/>
+      <c r="A170" s="93"/>
       <c r="G170" s="19"/>
       <c r="H170" s="19"/>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="94"/>
+      <c r="A171" s="93"/>
       <c r="G171" s="19"/>
       <c r="H171" s="19"/>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="94"/>
+      <c r="A172" s="93"/>
       <c r="G172" s="19"/>
       <c r="H172" s="19"/>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="94"/>
+      <c r="A173" s="93"/>
       <c r="G173" s="19"/>
       <c r="H173" s="19"/>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="94"/>
+      <c r="A174" s="93"/>
       <c r="G174" s="19"/>
       <c r="H174" s="19"/>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="94"/>
+      <c r="A175" s="93"/>
       <c r="G175" s="19"/>
       <c r="H175" s="19"/>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="94"/>
+      <c r="A176" s="93"/>
       <c r="G176" s="19"/>
       <c r="H176" s="19"/>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="94"/>
+      <c r="A177" s="93"/>
       <c r="G177" s="19"/>
       <c r="H177" s="19"/>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="94"/>
+      <c r="A178" s="93"/>
       <c r="G178" s="19"/>
       <c r="H178" s="19"/>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="94"/>
+      <c r="A179" s="93"/>
       <c r="G179" s="19"/>
       <c r="H179" s="19"/>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="94"/>
+      <c r="A180" s="93"/>
       <c r="G180" s="19"/>
       <c r="H180" s="19"/>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="94"/>
+      <c r="A181" s="93"/>
       <c r="G181" s="19"/>
       <c r="H181" s="19"/>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="94"/>
+      <c r="A182" s="93"/>
       <c r="G182" s="19"/>
       <c r="H182" s="19"/>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="94"/>
+      <c r="A183" s="93"/>
       <c r="G183" s="19"/>
       <c r="H183" s="19"/>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="94"/>
+      <c r="A184" s="93"/>
       <c r="G184" s="19"/>
       <c r="H184" s="19"/>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="94"/>
+      <c r="A185" s="93"/>
       <c r="G185" s="19"/>
       <c r="H185" s="19"/>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="94"/>
+      <c r="A186" s="93"/>
       <c r="G186" s="19"/>
       <c r="H186" s="19"/>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="94"/>
+      <c r="A187" s="93"/>
       <c r="G187" s="19"/>
       <c r="H187" s="19"/>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="94"/>
+      <c r="A188" s="93"/>
       <c r="G188" s="19"/>
       <c r="H188" s="19"/>
     </row>
     <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A189" s="94"/>
+      <c r="A189" s="93"/>
       <c r="G189" s="19"/>
       <c r="H189" s="19"/>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="94"/>
+      <c r="A190" s="93"/>
       <c r="G190" s="19"/>
       <c r="H190" s="19"/>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="94"/>
+      <c r="A191" s="93"/>
       <c r="G191" s="19"/>
       <c r="H191" s="19"/>
     </row>
     <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="94"/>
+      <c r="A192" s="93"/>
       <c r="G192" s="19"/>
       <c r="H192" s="19"/>
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="94"/>
+      <c r="A193" s="93"/>
       <c r="G193" s="19"/>
       <c r="H193" s="19"/>
     </row>
     <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A194" s="94"/>
+      <c r="A194" s="93"/>
       <c r="G194" s="19"/>
       <c r="H194" s="19"/>
     </row>
     <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A195" s="94"/>
+      <c r="A195" s="93"/>
       <c r="G195" s="19"/>
       <c r="H195" s="19"/>
     </row>
     <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="94"/>
+      <c r="A196" s="93"/>
       <c r="G196" s="19"/>
       <c r="H196" s="19"/>
     </row>
     <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="94"/>
+      <c r="A197" s="93"/>
       <c r="G197" s="19"/>
       <c r="H197" s="19"/>
     </row>
     <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="94"/>
+      <c r="A198" s="93"/>
       <c r="G198" s="19"/>
       <c r="H198" s="19"/>
     </row>
     <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A199" s="94"/>
+      <c r="A199" s="93"/>
       <c r="G199" s="19"/>
       <c r="H199" s="19"/>
     </row>
     <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="94"/>
+      <c r="A200" s="93"/>
       <c r="G200" s="19"/>
       <c r="H200" s="19"/>
     </row>
     <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A201" s="94"/>
+      <c r="A201" s="93"/>
       <c r="G201" s="19"/>
       <c r="H201" s="19"/>
     </row>
     <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="94"/>
+      <c r="A202" s="93"/>
       <c r="G202" s="19"/>
       <c r="H202" s="19"/>
     </row>
     <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="94"/>
+      <c r="A203" s="93"/>
       <c r="G203" s="19"/>
       <c r="H203" s="19"/>
     </row>
     <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A204" s="94"/>
+      <c r="A204" s="93"/>
       <c r="G204" s="19"/>
       <c r="H204" s="19"/>
     </row>
     <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A205" s="94"/>
+      <c r="A205" s="93"/>
       <c r="G205" s="19"/>
       <c r="H205" s="19"/>
     </row>
     <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A206" s="94"/>
+      <c r="A206" s="93"/>
       <c r="G206" s="19"/>
       <c r="H206" s="19"/>
     </row>
     <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="94"/>
+      <c r="A207" s="93"/>
       <c r="G207" s="19"/>
       <c r="H207" s="19"/>
     </row>
     <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="94"/>
+      <c r="A208" s="93"/>
       <c r="G208" s="19"/>
       <c r="H208" s="19"/>
     </row>
     <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A209" s="94"/>
+      <c r="A209" s="93"/>
       <c r="G209" s="19"/>
       <c r="H209" s="19"/>
     </row>
     <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A210" s="94"/>
+      <c r="A210" s="93"/>
       <c r="G210" s="19"/>
       <c r="H210" s="19"/>
     </row>
     <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A211" s="94"/>
+      <c r="A211" s="93"/>
       <c r="G211" s="19"/>
       <c r="H211" s="19"/>
     </row>
     <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A212" s="94"/>
+      <c r="A212" s="93"/>
       <c r="G212" s="19"/>
       <c r="H212" s="19"/>
     </row>
     <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A213" s="94"/>
+      <c r="A213" s="93"/>
       <c r="G213" s="19"/>
       <c r="H213" s="19"/>
     </row>
     <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A214" s="94"/>
+      <c r="A214" s="93"/>
       <c r="G214" s="19"/>
       <c r="H214" s="19"/>
     </row>
     <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A215" s="94"/>
+      <c r="A215" s="93"/>
       <c r="G215" s="19"/>
       <c r="H215" s="19"/>
     </row>
     <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A216" s="94"/>
+      <c r="A216" s="93"/>
       <c r="G216" s="19"/>
       <c r="H216" s="19"/>
     </row>
     <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A217" s="94"/>
+      <c r="A217" s="93"/>
       <c r="G217" s="19"/>
       <c r="H217" s="19"/>
     </row>
     <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A218" s="94"/>
+      <c r="A218" s="93"/>
       <c r="G218" s="19"/>
       <c r="H218" s="19"/>
     </row>
     <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A219" s="94"/>
+      <c r="A219" s="93"/>
       <c r="G219" s="19"/>
       <c r="H219" s="19"/>
     </row>
     <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A220" s="94"/>
+      <c r="A220" s="93"/>
       <c r="G220" s="19"/>
       <c r="H220" s="19"/>
     </row>
     <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A221" s="94"/>
+      <c r="A221" s="93"/>
       <c r="G221" s="19"/>
       <c r="H221" s="19"/>
     </row>
     <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A222" s="94"/>
+      <c r="A222" s="93"/>
       <c r="G222" s="19"/>
       <c r="H222" s="19"/>
     </row>
     <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A223" s="94"/>
+      <c r="A223" s="93"/>
       <c r="G223" s="19"/>
       <c r="H223" s="19"/>
     </row>
     <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A224" s="94"/>
+      <c r="A224" s="93"/>
       <c r="G224" s="19"/>
       <c r="H224" s="19"/>
     </row>
     <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A225" s="94"/>
+      <c r="A225" s="93"/>
       <c r="G225" s="19"/>
       <c r="H225" s="19"/>
     </row>
     <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A226" s="94"/>
+      <c r="A226" s="93"/>
       <c r="G226" s="19"/>
       <c r="H226" s="19"/>
     </row>
     <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A227" s="94"/>
+      <c r="A227" s="93"/>
       <c r="G227" s="19"/>
       <c r="H227" s="19"/>
     </row>
     <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A228" s="94"/>
+      <c r="A228" s="93"/>
       <c r="G228" s="19"/>
       <c r="H228" s="19"/>
     </row>
     <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A229" s="94"/>
+      <c r="A229" s="93"/>
       <c r="G229" s="19"/>
       <c r="H229" s="19"/>
     </row>
     <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A230" s="94"/>
+      <c r="A230" s="93"/>
       <c r="G230" s="19"/>
       <c r="H230" s="19"/>
     </row>
     <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A231" s="94"/>
+      <c r="A231" s="93"/>
       <c r="G231" s="19"/>
       <c r="H231" s="19"/>
     </row>
     <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A232" s="94"/>
+      <c r="A232" s="93"/>
       <c r="G232" s="19"/>
       <c r="H232" s="19"/>
     </row>
     <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A233" s="94"/>
+      <c r="A233" s="93"/>
       <c r="G233" s="19"/>
       <c r="H233" s="19"/>
     </row>
     <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A234" s="94"/>
+      <c r="A234" s="93"/>
       <c r="G234" s="19"/>
       <c r="H234" s="19"/>
     </row>
     <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A235" s="94"/>
+      <c r="A235" s="93"/>
       <c r="G235" s="19"/>
       <c r="H235" s="19"/>
     </row>
     <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A236" s="94"/>
+      <c r="A236" s="93"/>
       <c r="G236" s="19"/>
       <c r="H236" s="19"/>
     </row>
@@ -13718,7 +13708,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.73"/>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="4" min="3" style="0" width="12.63"/>
@@ -13727,7 +13717,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="94" t="s">
         <v>31</v>
       </c>
       <c r="B1" s="18" t="s">
@@ -13821,26 +13811,26 @@
       <c r="F5" s="19" t="s">
         <v>699</v>
       </c>
-      <c r="G5" s="96"/>
-      <c r="H5" s="96"/>
-      <c r="I5" s="96"/>
-      <c r="J5" s="96"/>
-      <c r="K5" s="96"/>
-      <c r="L5" s="96"/>
-      <c r="M5" s="96"/>
-      <c r="N5" s="96"/>
-      <c r="O5" s="96"/>
-      <c r="P5" s="96"/>
-      <c r="Q5" s="96"/>
-      <c r="R5" s="96"/>
-      <c r="S5" s="96"/>
-      <c r="T5" s="96"/>
-      <c r="U5" s="96"/>
-      <c r="V5" s="96"/>
-      <c r="W5" s="96"/>
-      <c r="X5" s="96"/>
-      <c r="Y5" s="96"/>
-      <c r="Z5" s="96"/>
+      <c r="G5" s="95"/>
+      <c r="H5" s="95"/>
+      <c r="I5" s="95"/>
+      <c r="J5" s="95"/>
+      <c r="K5" s="95"/>
+      <c r="L5" s="95"/>
+      <c r="M5" s="95"/>
+      <c r="N5" s="95"/>
+      <c r="O5" s="95"/>
+      <c r="P5" s="95"/>
+      <c r="Q5" s="95"/>
+      <c r="R5" s="95"/>
+      <c r="S5" s="95"/>
+      <c r="T5" s="95"/>
+      <c r="U5" s="95"/>
+      <c r="V5" s="95"/>
+      <c r="W5" s="95"/>
+      <c r="X5" s="95"/>
+      <c r="Y5" s="95"/>
+      <c r="Z5" s="95"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
@@ -13849,7 +13839,7 @@
       <c r="B6" s="19" t="s">
         <v>469</v>
       </c>
-      <c r="C6" s="97" t="s">
+      <c r="C6" s="96" t="s">
         <v>470</v>
       </c>
       <c r="D6" s="3"/>
@@ -13859,26 +13849,26 @@
       <c r="F6" s="19" t="s">
         <v>701</v>
       </c>
-      <c r="G6" s="96"/>
-      <c r="H6" s="96"/>
-      <c r="I6" s="96"/>
-      <c r="J6" s="96"/>
-      <c r="K6" s="96"/>
-      <c r="L6" s="96"/>
-      <c r="M6" s="96"/>
-      <c r="N6" s="96"/>
-      <c r="O6" s="96"/>
-      <c r="P6" s="96"/>
-      <c r="Q6" s="96"/>
-      <c r="R6" s="96"/>
-      <c r="S6" s="96"/>
-      <c r="T6" s="96"/>
-      <c r="U6" s="96"/>
-      <c r="V6" s="96"/>
-      <c r="W6" s="96"/>
-      <c r="X6" s="96"/>
-      <c r="Y6" s="96"/>
-      <c r="Z6" s="96"/>
+      <c r="G6" s="95"/>
+      <c r="H6" s="95"/>
+      <c r="I6" s="95"/>
+      <c r="J6" s="95"/>
+      <c r="K6" s="95"/>
+      <c r="L6" s="95"/>
+      <c r="M6" s="95"/>
+      <c r="N6" s="95"/>
+      <c r="O6" s="95"/>
+      <c r="P6" s="95"/>
+      <c r="Q6" s="95"/>
+      <c r="R6" s="95"/>
+      <c r="S6" s="95"/>
+      <c r="T6" s="95"/>
+      <c r="U6" s="95"/>
+      <c r="V6" s="95"/>
+      <c r="W6" s="95"/>
+      <c r="X6" s="95"/>
+      <c r="Y6" s="95"/>
+      <c r="Z6" s="95"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="14" t="s">
@@ -17903,14 +17893,14 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.75"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="98" t="s">
+      <c r="A2" s="97" t="s">
         <v>704</v>
       </c>
       <c r="B2" s="19" t="s">
@@ -17918,7 +17908,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="99" t="s">
+      <c r="A3" s="98" t="s">
         <v>706</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -17926,7 +17916,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="100" t="s">
+      <c r="A4" s="99" t="s">
         <v>708</v>
       </c>
     </row>
@@ -17968,23 +17958,23 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="101"/>
+      <c r="A13" s="100"/>
       <c r="B13" s="28" t="s">
         <v>716</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="102" t="s">
+      <c r="B14" s="101" t="s">
         <v>717</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="71" t="s">
+      <c r="B15" s="70" t="s">
         <v>718</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="103" t="s">
+      <c r="B16" s="102" t="s">
         <v>719</v>
       </c>
     </row>
@@ -17996,7 +17986,7 @@
       <c r="A18" s="1" t="s">
         <v>720</v>
       </c>
-      <c r="B18" s="104" t="s">
+      <c r="B18" s="103" t="s">
         <v>721</v>
       </c>
     </row>
@@ -18004,13 +17994,13 @@
       <c r="A19" s="3" t="s">
         <v>722</v>
       </c>
-      <c r="B19" s="71"/>
+      <c r="B19" s="70"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>723</v>
       </c>
-      <c r="B21" s="105" t="s">
+      <c r="B21" s="104" t="s">
         <v>724</v>
       </c>
     </row>
@@ -18038,7 +18028,7 @@
       <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.38"/>
   </cols>
@@ -18127,7 +18117,7 @@
       <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.25"/>
   </cols>
@@ -18212,7 +18202,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="19"/>
@@ -18239,7 +18229,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="81.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.13"/>
@@ -18248,14 +18238,14 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="105" t="s">
         <v>747</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106" t="s">
+      <c r="B1" s="105"/>
+      <c r="C1" s="105" t="s">
         <v>748</v>
       </c>
-      <c r="D1" s="106"/>
+      <c r="D1" s="105"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -18281,7 +18271,7 @@
       <c r="C3" s="3" t="s">
         <v>755</v>
       </c>
-      <c r="D3" s="107" t="str">
+      <c r="D3" s="106" t="str">
         <f aca="false">RIGHT(A3,LEN(A3) - (FIND(" == ",A3) + 3))</f>
         <v>ADDRESS_CONTRACTING_BODY</v>
       </c>
@@ -18333,7 +18323,7 @@
       <c r="C7" s="3" t="s">
         <v>755</v>
       </c>
-      <c r="D7" s="108" t="s">
+      <c r="D7" s="107" t="s">
         <v>763</v>
       </c>
     </row>
@@ -18347,7 +18337,7 @@
       <c r="C8" s="3" t="s">
         <v>755</v>
       </c>
-      <c r="D8" s="109" t="s">
+      <c r="D8" s="108" t="s">
         <v>766</v>
       </c>
     </row>
@@ -18391,7 +18381,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="70.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.38"/>
@@ -18400,10 +18390,10 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="105" t="s">
         <v>747</v>
       </c>
-      <c r="B1" s="106"/>
+      <c r="B1" s="105"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -18442,7 +18432,7 @@
       <c r="B5" s="3" t="s">
         <v>775</v>
       </c>
-      <c r="C5" s="109" t="s">
+      <c r="C5" s="108" t="s">
         <v>773</v>
       </c>
       <c r="D5" s="3" t="s">

</xml_diff>

<commit_message>
Generated output and validation reports for form F25.
</commit_message>
<xml_diff>
--- a/mappings/package_F25/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_F25/transformation/conceptual_mappings.xlsx
@@ -398,7 +398,7 @@
     <t>Mapping Version</t>
   </si>
   <si>
-    <t>4.2.1</t>
+    <t>5.1.0</t>
   </si>
   <si>
     <r>
@@ -564,7 +564,7 @@
     <t>CONTRACTING_BODY/ADDRESS_CONTRACTING_BODY</t>
   </si>
   <si>
-    <t>epo:ResultNotice / epo:AgentInRole (from CL1)</t>
+    <t>epo:Notice / epo:AgentInRole (from CL1)</t>
   </si>
   <si>
     <t>?this epo:refersToRole ?value</t>
@@ -1928,7 +1928,7 @@
     <t>OBJECT_CONTRACT</t>
   </si>
   <si>
-    <t>epo:ResultNotice / epo:NoticeAwardInformation</t>
+    <t>epo:Notice / epo:NoticeAwardInformation</t>
   </si>
   <si>
     <t>?this epo:announcesNoticeAwardInformation ?value .</t>
@@ -1943,7 +1943,7 @@
     <t>OBJECT_CONTRACT/VAL_TOTAL</t>
   </si>
   <si>
-    <t>epo:ResultNotice / epo:NoticeAwardInformation / epo:MonetaryValue / xsd:decimal</t>
+    <t>epo:Notice / epo:NoticeAwardInformation / epo:MonetaryValue / xsd:decimal</t>
   </si>
   <si>
     <t>?this epo:announcesNoticeAwardInformation / epo:hasTotalAwardedValue / epo:hasAmountValue ?value .</t>
@@ -2027,7 +2027,7 @@
     <t>OBJECT_CONTRACT/VAL_TOTAL/@CURRENCY</t>
   </si>
   <si>
-    <t>epo:ResultNotice / epo:NoticeAwardInformation / epo:MonetaryValue / at-voc:currency (from currency.json)</t>
+    <t>epo:Notice / epo:NoticeAwardInformation / epo:MonetaryValue / at-voc:currency (from currency.json)</t>
   </si>
   <si>
     <r>
@@ -2067,7 +2067,7 @@
     <t>II.2</t>
   </si>
   <si>
-    <t>epo:ResultNotice / epo:Lot</t>
+    <t>epo:Notice / epo:Lot</t>
   </si>
   <si>
     <t>?this epo:refersToLot ?value .</t>
@@ -2766,7 +2766,7 @@
     <t>PROCEDURE/NOTICE_NUMBER_OJ</t>
   </si>
   <si>
-    <t>epo:ResultNotice / epo:Notice /  epo:Identifier / xsd:string</t>
+    <t>epo:Notice / epo:Notice /  epo:Identifier / xsd:string</t>
   </si>
   <si>
     <r>
@@ -4329,7 +4329,7 @@
     <t>COMPLEMENTARY_INFO/ADDRESS_MEDIATION_BODY</t>
   </si>
   <si>
-    <t>epo:ResultNotice / epo:Mediator</t>
+    <t>epo:Notice / epo:Mediator</t>
   </si>
   <si>
     <t>VI.4.2.1</t>
@@ -4915,7 +4915,7 @@
     <t>COMPLEMENTARY_INFO/DATE_DISPATCH_NOTICE</t>
   </si>
   <si>
-    <t>epo:ResultNotice</t>
+    <t>epo:Notice</t>
   </si>
   <si>
     <r>
@@ -5360,7 +5360,7 @@
     <t>annex_d4.rml.ttl</t>
   </si>
   <si>
-    <t>result_notice.rml.ttl</t>
+    <t>notice.rml.ttl</t>
   </si>
   <si>
     <t>Informal (if possible to become formal)</t>
@@ -5841,7 +5841,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="163">
+  <cellXfs count="164">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -6306,6 +6306,9 @@
     <xf borderId="10" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="10" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
@@ -19047,7 +19050,7 @@
       <c r="B8" s="6"/>
     </row>
     <row r="9">
-      <c r="A9" s="157" t="s">
+      <c r="A9" s="158" t="s">
         <v>801</v>
       </c>
       <c r="B9" s="6"/>
@@ -19092,10 +19095,10 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="158" t="s">
+      <c r="A1" s="159" t="s">
         <v>802</v>
       </c>
-      <c r="C1" s="158" t="s">
+      <c r="C1" s="159" t="s">
         <v>803</v>
       </c>
     </row>
@@ -19267,7 +19270,7 @@
       <c r="C7" s="4" t="s">
         <v>810</v>
       </c>
-      <c r="D7" s="159" t="s">
+      <c r="D7" s="160" t="s">
         <v>819</v>
       </c>
       <c r="E7" s="6"/>
@@ -19330,220 +19333,220 @@
       <c r="Z8" s="6"/>
     </row>
     <row r="9">
-      <c r="A9" s="160" t="s">
+      <c r="A9" s="161" t="s">
         <v>823</v>
       </c>
-      <c r="B9" s="161" t="s">
+      <c r="B9" s="162" t="s">
         <v>824</v>
       </c>
-      <c r="C9" s="161" t="s">
+      <c r="C9" s="162" t="s">
         <v>810</v>
       </c>
-      <c r="D9" s="161" t="s">
+      <c r="D9" s="162" t="s">
         <v>825</v>
       </c>
-      <c r="E9" s="161"/>
-      <c r="F9" s="161"/>
-      <c r="G9" s="161"/>
-      <c r="H9" s="161"/>
-      <c r="I9" s="161"/>
-      <c r="J9" s="161"/>
-      <c r="K9" s="161"/>
-      <c r="L9" s="161"/>
-      <c r="M9" s="161"/>
-      <c r="N9" s="161"/>
-      <c r="O9" s="161"/>
-      <c r="P9" s="161"/>
-      <c r="Q9" s="161"/>
-      <c r="R9" s="161"/>
-      <c r="S9" s="161"/>
-      <c r="T9" s="161"/>
-      <c r="U9" s="161"/>
-      <c r="V9" s="161"/>
-      <c r="W9" s="161"/>
-      <c r="X9" s="161"/>
-      <c r="Y9" s="161"/>
-      <c r="Z9" s="161"/>
+      <c r="E9" s="162"/>
+      <c r="F9" s="162"/>
+      <c r="G9" s="162"/>
+      <c r="H9" s="162"/>
+      <c r="I9" s="162"/>
+      <c r="J9" s="162"/>
+      <c r="K9" s="162"/>
+      <c r="L9" s="162"/>
+      <c r="M9" s="162"/>
+      <c r="N9" s="162"/>
+      <c r="O9" s="162"/>
+      <c r="P9" s="162"/>
+      <c r="Q9" s="162"/>
+      <c r="R9" s="162"/>
+      <c r="S9" s="162"/>
+      <c r="T9" s="162"/>
+      <c r="U9" s="162"/>
+      <c r="V9" s="162"/>
+      <c r="W9" s="162"/>
+      <c r="X9" s="162"/>
+      <c r="Y9" s="162"/>
+      <c r="Z9" s="162"/>
     </row>
     <row r="10">
-      <c r="A10" s="160" t="s">
+      <c r="A10" s="161" t="s">
         <v>826</v>
       </c>
-      <c r="B10" s="161" t="s">
+      <c r="B10" s="162" t="s">
         <v>824</v>
       </c>
-      <c r="C10" s="161" t="s">
+      <c r="C10" s="162" t="s">
         <v>810</v>
       </c>
-      <c r="D10" s="161" t="s">
+      <c r="D10" s="162" t="s">
         <v>827</v>
       </c>
-      <c r="E10" s="161"/>
-      <c r="F10" s="161"/>
-      <c r="G10" s="161"/>
-      <c r="H10" s="161"/>
-      <c r="I10" s="161"/>
-      <c r="J10" s="161"/>
-      <c r="K10" s="161"/>
-      <c r="L10" s="161"/>
-      <c r="M10" s="161"/>
-      <c r="N10" s="161"/>
-      <c r="O10" s="161"/>
-      <c r="P10" s="161"/>
-      <c r="Q10" s="161"/>
-      <c r="R10" s="161"/>
-      <c r="S10" s="161"/>
-      <c r="T10" s="161"/>
-      <c r="U10" s="161"/>
-      <c r="V10" s="161"/>
-      <c r="W10" s="161"/>
-      <c r="X10" s="161"/>
-      <c r="Y10" s="161"/>
-      <c r="Z10" s="161"/>
+      <c r="E10" s="162"/>
+      <c r="F10" s="162"/>
+      <c r="G10" s="162"/>
+      <c r="H10" s="162"/>
+      <c r="I10" s="162"/>
+      <c r="J10" s="162"/>
+      <c r="K10" s="162"/>
+      <c r="L10" s="162"/>
+      <c r="M10" s="162"/>
+      <c r="N10" s="162"/>
+      <c r="O10" s="162"/>
+      <c r="P10" s="162"/>
+      <c r="Q10" s="162"/>
+      <c r="R10" s="162"/>
+      <c r="S10" s="162"/>
+      <c r="T10" s="162"/>
+      <c r="U10" s="162"/>
+      <c r="V10" s="162"/>
+      <c r="W10" s="162"/>
+      <c r="X10" s="162"/>
+      <c r="Y10" s="162"/>
+      <c r="Z10" s="162"/>
     </row>
     <row r="11">
-      <c r="A11" s="160" t="s">
+      <c r="A11" s="161" t="s">
         <v>828</v>
       </c>
-      <c r="B11" s="161" t="s">
+      <c r="B11" s="162" t="s">
         <v>829</v>
       </c>
-      <c r="C11" s="161" t="s">
+      <c r="C11" s="162" t="s">
         <v>810</v>
       </c>
-      <c r="D11" s="161" t="s">
+      <c r="D11" s="162" t="s">
         <v>830</v>
       </c>
-      <c r="E11" s="161"/>
-      <c r="F11" s="161"/>
-      <c r="G11" s="161"/>
-      <c r="H11" s="161"/>
-      <c r="I11" s="161"/>
-      <c r="J11" s="161"/>
-      <c r="K11" s="161"/>
-      <c r="L11" s="161"/>
-      <c r="M11" s="161"/>
-      <c r="N11" s="161"/>
-      <c r="O11" s="161"/>
-      <c r="P11" s="161"/>
-      <c r="Q11" s="161"/>
-      <c r="R11" s="161"/>
-      <c r="S11" s="161"/>
-      <c r="T11" s="161"/>
-      <c r="U11" s="161"/>
-      <c r="V11" s="161"/>
-      <c r="W11" s="161"/>
-      <c r="X11" s="161"/>
-      <c r="Y11" s="161"/>
-      <c r="Z11" s="161"/>
+      <c r="E11" s="162"/>
+      <c r="F11" s="162"/>
+      <c r="G11" s="162"/>
+      <c r="H11" s="162"/>
+      <c r="I11" s="162"/>
+      <c r="J11" s="162"/>
+      <c r="K11" s="162"/>
+      <c r="L11" s="162"/>
+      <c r="M11" s="162"/>
+      <c r="N11" s="162"/>
+      <c r="O11" s="162"/>
+      <c r="P11" s="162"/>
+      <c r="Q11" s="162"/>
+      <c r="R11" s="162"/>
+      <c r="S11" s="162"/>
+      <c r="T11" s="162"/>
+      <c r="U11" s="162"/>
+      <c r="V11" s="162"/>
+      <c r="W11" s="162"/>
+      <c r="X11" s="162"/>
+      <c r="Y11" s="162"/>
+      <c r="Z11" s="162"/>
     </row>
     <row r="12">
-      <c r="A12" s="160" t="s">
+      <c r="A12" s="161" t="s">
         <v>831</v>
       </c>
-      <c r="B12" s="161" t="s">
+      <c r="B12" s="162" t="s">
         <v>829</v>
       </c>
-      <c r="C12" s="161" t="s">
+      <c r="C12" s="162" t="s">
         <v>810</v>
       </c>
-      <c r="D12" s="161" t="s">
+      <c r="D12" s="162" t="s">
         <v>832</v>
       </c>
-      <c r="E12" s="161"/>
-      <c r="F12" s="161"/>
-      <c r="G12" s="161"/>
-      <c r="H12" s="161"/>
-      <c r="I12" s="161"/>
-      <c r="J12" s="161"/>
-      <c r="K12" s="161"/>
-      <c r="L12" s="161"/>
-      <c r="M12" s="161"/>
-      <c r="N12" s="161"/>
-      <c r="O12" s="161"/>
-      <c r="P12" s="161"/>
-      <c r="Q12" s="161"/>
-      <c r="R12" s="161"/>
-      <c r="S12" s="161"/>
-      <c r="T12" s="161"/>
-      <c r="U12" s="161"/>
-      <c r="V12" s="161"/>
-      <c r="W12" s="161"/>
-      <c r="X12" s="161"/>
-      <c r="Y12" s="161"/>
-      <c r="Z12" s="161"/>
+      <c r="E12" s="162"/>
+      <c r="F12" s="162"/>
+      <c r="G12" s="162"/>
+      <c r="H12" s="162"/>
+      <c r="I12" s="162"/>
+      <c r="J12" s="162"/>
+      <c r="K12" s="162"/>
+      <c r="L12" s="162"/>
+      <c r="M12" s="162"/>
+      <c r="N12" s="162"/>
+      <c r="O12" s="162"/>
+      <c r="P12" s="162"/>
+      <c r="Q12" s="162"/>
+      <c r="R12" s="162"/>
+      <c r="S12" s="162"/>
+      <c r="T12" s="162"/>
+      <c r="U12" s="162"/>
+      <c r="V12" s="162"/>
+      <c r="W12" s="162"/>
+      <c r="X12" s="162"/>
+      <c r="Y12" s="162"/>
+      <c r="Z12" s="162"/>
     </row>
     <row r="13">
-      <c r="A13" s="160" t="s">
+      <c r="A13" s="161" t="s">
         <v>833</v>
       </c>
-      <c r="B13" s="160" t="s">
+      <c r="B13" s="161" t="s">
         <v>813</v>
       </c>
-      <c r="C13" s="161" t="s">
+      <c r="C13" s="162" t="s">
         <v>810</v>
       </c>
-      <c r="D13" s="161" t="s">
+      <c r="D13" s="162" t="s">
         <v>834</v>
       </c>
-      <c r="E13" s="161"/>
-      <c r="F13" s="161"/>
-      <c r="G13" s="161"/>
-      <c r="H13" s="161"/>
-      <c r="I13" s="161"/>
-      <c r="J13" s="161"/>
-      <c r="K13" s="161"/>
-      <c r="L13" s="161"/>
-      <c r="M13" s="161"/>
-      <c r="N13" s="161"/>
-      <c r="O13" s="161"/>
-      <c r="P13" s="161"/>
-      <c r="Q13" s="161"/>
-      <c r="R13" s="161"/>
-      <c r="S13" s="161"/>
-      <c r="T13" s="161"/>
-      <c r="U13" s="161"/>
-      <c r="V13" s="161"/>
-      <c r="W13" s="161"/>
-      <c r="X13" s="161"/>
-      <c r="Y13" s="161"/>
-      <c r="Z13" s="161"/>
+      <c r="E13" s="162"/>
+      <c r="F13" s="162"/>
+      <c r="G13" s="162"/>
+      <c r="H13" s="162"/>
+      <c r="I13" s="162"/>
+      <c r="J13" s="162"/>
+      <c r="K13" s="162"/>
+      <c r="L13" s="162"/>
+      <c r="M13" s="162"/>
+      <c r="N13" s="162"/>
+      <c r="O13" s="162"/>
+      <c r="P13" s="162"/>
+      <c r="Q13" s="162"/>
+      <c r="R13" s="162"/>
+      <c r="S13" s="162"/>
+      <c r="T13" s="162"/>
+      <c r="U13" s="162"/>
+      <c r="V13" s="162"/>
+      <c r="W13" s="162"/>
+      <c r="X13" s="162"/>
+      <c r="Y13" s="162"/>
+      <c r="Z13" s="162"/>
     </row>
     <row r="14">
-      <c r="A14" s="160" t="s">
+      <c r="A14" s="161" t="s">
         <v>835</v>
       </c>
-      <c r="B14" s="160" t="s">
+      <c r="B14" s="161" t="s">
         <v>813</v>
       </c>
-      <c r="C14" s="161" t="s">
+      <c r="C14" s="162" t="s">
         <v>810</v>
       </c>
-      <c r="D14" s="161" t="s">
+      <c r="D14" s="162" t="s">
         <v>836</v>
       </c>
-      <c r="E14" s="161"/>
-      <c r="F14" s="161"/>
-      <c r="G14" s="161"/>
-      <c r="H14" s="161"/>
-      <c r="I14" s="161"/>
-      <c r="J14" s="161"/>
-      <c r="K14" s="161"/>
-      <c r="L14" s="161"/>
-      <c r="M14" s="161"/>
-      <c r="N14" s="161"/>
-      <c r="O14" s="161"/>
-      <c r="P14" s="161"/>
-      <c r="Q14" s="161"/>
-      <c r="R14" s="161"/>
-      <c r="S14" s="161"/>
-      <c r="T14" s="161"/>
-      <c r="U14" s="161"/>
-      <c r="V14" s="161"/>
-      <c r="W14" s="161"/>
-      <c r="X14" s="161"/>
-      <c r="Y14" s="161"/>
-      <c r="Z14" s="161"/>
+      <c r="E14" s="162"/>
+      <c r="F14" s="162"/>
+      <c r="G14" s="162"/>
+      <c r="H14" s="162"/>
+      <c r="I14" s="162"/>
+      <c r="J14" s="162"/>
+      <c r="K14" s="162"/>
+      <c r="L14" s="162"/>
+      <c r="M14" s="162"/>
+      <c r="N14" s="162"/>
+      <c r="O14" s="162"/>
+      <c r="P14" s="162"/>
+      <c r="Q14" s="162"/>
+      <c r="R14" s="162"/>
+      <c r="S14" s="162"/>
+      <c r="T14" s="162"/>
+      <c r="U14" s="162"/>
+      <c r="V14" s="162"/>
+      <c r="W14" s="162"/>
+      <c r="X14" s="162"/>
+      <c r="Y14" s="162"/>
+      <c r="Z14" s="162"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -19571,7 +19574,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="158" t="s">
+      <c r="A1" s="159" t="s">
         <v>802</v>
       </c>
     </row>
@@ -19612,7 +19615,7 @@
       <c r="B5" s="142" t="s">
         <v>842</v>
       </c>
-      <c r="C5" s="162" t="s">
+      <c r="C5" s="163" t="s">
         <v>840</v>
       </c>
       <c r="D5" s="142" t="s">

</xml_diff>

<commit_message>
Generated output for F23 and F25 after fixing issue #217, and with CM version 5.1.1
</commit_message>
<xml_diff>
--- a/mappings/package_F25/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_F25/transformation/conceptual_mappings.xlsx
@@ -363,7 +363,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1159" uniqueCount="844">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1161" uniqueCount="846">
   <si>
     <t>Field</t>
   </si>
@@ -398,7 +398,7 @@
     <t>Mapping Version</t>
   </si>
   <si>
-    <t>5.1.0</t>
+    <t>5.1.1</t>
   </si>
   <si>
     <r>
@@ -422,7 +422,7 @@
     <t>EPO version</t>
   </si>
   <si>
-    <t>3.1.0-dev</t>
+    <t>3.1.0</t>
   </si>
   <si>
     <r>
@@ -2660,6 +2660,41 @@
   </si>
   <si>
     <t>PROCEDURE/PT_AWARD_CONTRACT_WITHOUT_PUBLICATION</t>
+  </si>
+  <si>
+    <t>epo:Procedure / at-voc:procurement-procedure-type</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+      </rPr>
+      <t>?this</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+      </rPr>
+      <t xml:space="preserve"> epo:hasProcedureType &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>http://publications.europa.eu/resource/authority/procurement-procedure-type/neg-wo-call</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+      </rPr>
+      <t>&gt; .</t>
+    </r>
   </si>
   <si>
     <t>IV.1.8</t>
@@ -5496,7 +5531,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="33">
+  <fonts count="34">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -5569,6 +5604,12 @@
     <font>
       <b/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -5841,7 +5882,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="164">
+  <cellXfs count="165">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -6107,6 +6148,9 @@
     <xf borderId="0" fillId="6" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="4" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="8" fontId="14" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
@@ -6119,7 +6163,7 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -6128,10 +6172,10 @@
     <xf quotePrefix="1" borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf quotePrefix="1" borderId="0" fillId="10" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf quotePrefix="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -6140,7 +6184,7 @@
     <xf borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf quotePrefix="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -6161,13 +6205,13 @@
     <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="7" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="4" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="4" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="11" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -6176,7 +6220,7 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -6215,13 +6259,13 @@
     <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="4" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="4" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -6230,19 +6274,19 @@
     <xf quotePrefix="1" borderId="0" fillId="10" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="10" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="10" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="10" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="10" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf quotePrefix="1" borderId="0" fillId="10" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="10" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="10" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="10" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="10" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="9" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -6251,23 +6295,23 @@
     <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="28" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -6297,7 +6341,7 @@
     <xf borderId="0" fillId="9" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -6309,10 +6353,10 @@
     <xf borderId="10" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="32" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="15" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
@@ -6321,7 +6365,7 @@
     <xf borderId="0" fillId="15" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="32" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -11992,12 +12036,12 @@
       <c r="B71" s="47" t="s">
         <v>376</v>
       </c>
-      <c r="C71" s="56"/>
-      <c r="D71" s="56"/>
-      <c r="E71" s="56"/>
-      <c r="F71" s="56"/>
-      <c r="G71" s="56"/>
-      <c r="H71" s="56"/>
+      <c r="C71" s="4"/>
+      <c r="D71" s="4"/>
+      <c r="E71" s="39"/>
+      <c r="F71" s="4"/>
+      <c r="G71" s="4"/>
+      <c r="H71" s="4"/>
       <c r="I71" s="6"/>
       <c r="J71" s="6"/>
       <c r="K71" s="6"/>
@@ -12016,18 +12060,18 @@
       <c r="B72" s="55" t="s">
         <v>378</v>
       </c>
-      <c r="C72" s="70"/>
-      <c r="D72" s="70"/>
-      <c r="E72" s="57" t="s">
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="39" t="s">
         <v>379</v>
       </c>
-      <c r="F72" s="70" t="s">
+      <c r="F72" s="6" t="s">
         <v>380</v>
       </c>
-      <c r="G72" s="56" t="s">
+      <c r="G72" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="H72" s="56" t="s">
+      <c r="H72" s="4" t="s">
         <v>382</v>
       </c>
       <c r="I72" s="6"/>
@@ -12048,14 +12092,18 @@
       <c r="B73" s="55" t="s">
         <v>384</v>
       </c>
-      <c r="C73" s="56"/>
-      <c r="D73" s="56"/>
-      <c r="E73" s="57" t="s">
+      <c r="C73" s="4"/>
+      <c r="D73" s="4"/>
+      <c r="E73" s="39" t="s">
         <v>385</v>
       </c>
-      <c r="F73" s="70"/>
-      <c r="G73" s="56"/>
-      <c r="H73" s="56"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="36" t="s">
+        <v>386</v>
+      </c>
+      <c r="H73" s="91" t="s">
+        <v>387</v>
+      </c>
       <c r="I73" s="6"/>
       <c r="J73" s="6"/>
       <c r="K73" s="6"/>
@@ -12069,26 +12117,26 @@
     </row>
     <row r="74">
       <c r="A74" s="48" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="B74" s="47" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="C74" s="36" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="D74" s="49" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="E74" s="49" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="F74" s="36"/>
       <c r="G74" s="36" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="H74" s="73" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="I74" s="6"/>
       <c r="J74" s="6"/>
@@ -12102,27 +12150,27 @@
       <c r="R74" s="28"/>
     </row>
     <row r="75">
-      <c r="A75" s="91" t="s">
-        <v>386</v>
-      </c>
-      <c r="B75" s="92" t="s">
-        <v>387</v>
+      <c r="A75" s="92" t="s">
+        <v>388</v>
+      </c>
+      <c r="B75" s="93" t="s">
+        <v>389</v>
       </c>
       <c r="C75" s="85" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="D75" s="86" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="E75" s="49" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="F75" s="36"/>
       <c r="G75" s="36" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="H75" s="73" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="I75" s="6"/>
       <c r="J75" s="6"/>
@@ -12137,10 +12185,10 @@
     </row>
     <row r="76">
       <c r="A76" s="90" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="B76" s="38" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="C76" s="4"/>
       <c r="D76" s="4"/>
@@ -12161,22 +12209,22 @@
     </row>
     <row r="77">
       <c r="A77" s="48" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="B77" s="47" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="C77" s="36"/>
       <c r="D77" s="36"/>
       <c r="E77" s="49" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="F77" s="13"/>
       <c r="G77" s="49" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="H77" s="73" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="I77" s="6"/>
       <c r="J77" s="6"/>
@@ -12191,22 +12239,22 @@
     </row>
     <row r="78">
       <c r="A78" s="89" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="B78" s="67" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="C78" s="4"/>
       <c r="D78" s="4"/>
-      <c r="E78" s="93" t="s">
-        <v>404</v>
+      <c r="E78" s="94" t="s">
+        <v>406</v>
       </c>
       <c r="F78" s="4"/>
       <c r="G78" s="4" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="H78" s="4" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="I78" s="6"/>
       <c r="J78" s="6"/>
@@ -12221,28 +12269,28 @@
     </row>
     <row r="79">
       <c r="A79" s="48" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="B79" s="47" t="s">
         <v>6</v>
       </c>
       <c r="C79" s="49" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="D79" s="49" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="E79" s="49" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="F79" s="49" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>412</v>
-      </c>
-      <c r="H79" s="94" t="s">
-        <v>413</v>
+        <v>414</v>
+      </c>
+      <c r="H79" s="95" t="s">
+        <v>415</v>
       </c>
       <c r="I79" s="6"/>
       <c r="J79" s="6"/>
@@ -12257,26 +12305,26 @@
     </row>
     <row r="80">
       <c r="A80" s="48" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="B80" s="47" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="C80" s="49" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="D80" s="49" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="E80" s="58" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="F80" s="4"/>
       <c r="G80" s="4" t="s">
-        <v>419</v>
-      </c>
-      <c r="H80" s="95" t="s">
-        <v>420</v>
+        <v>421</v>
+      </c>
+      <c r="H80" s="96" t="s">
+        <v>422</v>
       </c>
       <c r="I80" s="6"/>
       <c r="J80" s="6"/>
@@ -12290,27 +12338,27 @@
       <c r="R80" s="28"/>
     </row>
     <row r="81">
-      <c r="A81" s="91" t="s">
-        <v>414</v>
-      </c>
-      <c r="B81" s="92" t="s">
-        <v>415</v>
+      <c r="A81" s="92" t="s">
+        <v>416</v>
+      </c>
+      <c r="B81" s="93" t="s">
+        <v>417</v>
       </c>
       <c r="C81" s="86" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="D81" s="86" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="E81" s="58" t="s">
-        <v>418</v>
-      </c>
-      <c r="F81" s="96"/>
+        <v>420</v>
+      </c>
+      <c r="F81" s="97"/>
       <c r="G81" s="40" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="H81" s="40" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="I81" s="6"/>
       <c r="J81" s="6"/>
@@ -12324,27 +12372,27 @@
       <c r="R81" s="28"/>
     </row>
     <row r="82">
-      <c r="A82" s="91" t="s">
-        <v>414</v>
-      </c>
-      <c r="B82" s="92" t="s">
-        <v>415</v>
+      <c r="A82" s="92" t="s">
+        <v>416</v>
+      </c>
+      <c r="B82" s="93" t="s">
+        <v>417</v>
       </c>
       <c r="C82" s="86" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="D82" s="86" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="E82" s="58" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="F82" s="4"/>
       <c r="G82" s="4" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="H82" s="39" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="I82" s="6"/>
       <c r="J82" s="6"/>
@@ -12359,13 +12407,13 @@
     </row>
     <row r="83">
       <c r="A83" s="90" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="B83" s="38" t="s">
-        <v>427</v>
-      </c>
-      <c r="C83" s="97" t="s">
-        <v>428</v>
+        <v>429</v>
+      </c>
+      <c r="C83" s="98" t="s">
+        <v>430</v>
       </c>
       <c r="D83" s="49"/>
       <c r="E83" s="4"/>
@@ -12385,19 +12433,19 @@
     </row>
     <row r="84">
       <c r="A84" s="46" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="B84" s="47" t="s">
+        <v>432</v>
+      </c>
+      <c r="C84" s="99" t="s">
         <v>430</v>
       </c>
-      <c r="C84" s="98" t="s">
-        <v>428</v>
-      </c>
-      <c r="D84" s="57"/>
-      <c r="E84" s="56"/>
-      <c r="F84" s="56"/>
-      <c r="G84" s="56"/>
-      <c r="H84" s="56"/>
+      <c r="D84" s="39"/>
+      <c r="E84" s="4"/>
+      <c r="F84" s="4"/>
+      <c r="G84" s="4"/>
+      <c r="H84" s="4"/>
       <c r="I84" s="6"/>
       <c r="J84" s="6"/>
       <c r="K84" s="6"/>
@@ -12411,26 +12459,26 @@
     </row>
     <row r="85">
       <c r="A85" s="69" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="B85" s="55" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="C85" s="49" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="D85" s="49" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="E85" s="49" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="F85" s="49"/>
       <c r="G85" s="36" t="s">
-        <v>436</v>
-      </c>
-      <c r="H85" s="99" t="s">
-        <v>437</v>
+        <v>438</v>
+      </c>
+      <c r="H85" s="100" t="s">
+        <v>439</v>
       </c>
       <c r="I85" s="6"/>
       <c r="J85" s="6"/>
@@ -12445,26 +12493,26 @@
     </row>
     <row r="86">
       <c r="A86" s="69" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="B86" s="55" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="C86" s="49" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="D86" s="49" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="E86" s="49" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="F86" s="49"/>
       <c r="G86" s="4" t="s">
-        <v>436</v>
-      </c>
-      <c r="H86" s="95" t="s">
-        <v>441</v>
+        <v>438</v>
+      </c>
+      <c r="H86" s="96" t="s">
+        <v>443</v>
       </c>
       <c r="I86" s="6"/>
       <c r="J86" s="6"/>
@@ -12479,24 +12527,24 @@
     </row>
     <row r="87">
       <c r="A87" s="69" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="B87" s="55" t="s">
-        <v>443</v>
-      </c>
-      <c r="C87" s="100" t="s">
-        <v>444</v>
+        <v>445</v>
+      </c>
+      <c r="C87" s="101" t="s">
+        <v>446</v>
       </c>
       <c r="D87" s="49"/>
-      <c r="E87" s="101" t="s">
-        <v>445</v>
-      </c>
-      <c r="F87" s="101"/>
-      <c r="G87" s="101" t="s">
-        <v>446</v>
-      </c>
-      <c r="H87" s="102" t="s">
+      <c r="E87" s="102" t="s">
         <v>447</v>
+      </c>
+      <c r="F87" s="102"/>
+      <c r="G87" s="102" t="s">
+        <v>448</v>
+      </c>
+      <c r="H87" s="103" t="s">
+        <v>449</v>
       </c>
       <c r="I87" s="6"/>
       <c r="J87" s="6"/>
@@ -12504,13 +12552,13 @@
     </row>
     <row r="88">
       <c r="A88" s="90" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="B88" s="38" t="s">
-        <v>449</v>
-      </c>
-      <c r="C88" s="103" t="s">
-        <v>428</v>
+        <v>451</v>
+      </c>
+      <c r="C88" s="104" t="s">
+        <v>430</v>
       </c>
       <c r="D88" s="4"/>
       <c r="E88" s="4"/>
@@ -12523,20 +12571,20 @@
     </row>
     <row r="89">
       <c r="A89" s="69" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="B89" s="55"/>
       <c r="C89" s="49"/>
       <c r="D89" s="4"/>
       <c r="E89" s="58" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="F89" s="49"/>
       <c r="G89" s="36" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="H89" s="49" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="I89" s="6"/>
       <c r="J89" s="6"/>
@@ -12544,20 +12592,20 @@
     </row>
     <row r="90">
       <c r="A90" s="69" t="s">
-        <v>450</v>
-      </c>
-      <c r="B90" s="104"/>
+        <v>452</v>
+      </c>
+      <c r="B90" s="105"/>
       <c r="C90" s="49"/>
       <c r="D90" s="4"/>
       <c r="E90" s="58" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="F90" s="49"/>
       <c r="G90" s="36" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="H90" s="49" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="I90" s="6"/>
       <c r="J90" s="6"/>
@@ -12565,26 +12613,26 @@
     </row>
     <row r="91">
       <c r="A91" s="48" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="B91" s="47" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="E91" s="58" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="F91" s="6"/>
       <c r="G91" s="4" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="H91" s="39" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="I91" s="6"/>
       <c r="J91" s="6"/>
@@ -12592,22 +12640,22 @@
     </row>
     <row r="92">
       <c r="A92" s="48" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="B92" s="47" t="s">
-        <v>462</v>
-      </c>
-      <c r="C92" s="105"/>
-      <c r="D92" s="105"/>
-      <c r="E92" s="106" t="s">
-        <v>418</v>
-      </c>
-      <c r="F92" s="105"/>
+        <v>464</v>
+      </c>
+      <c r="C92" s="106"/>
+      <c r="D92" s="106"/>
+      <c r="E92" s="107" t="s">
+        <v>420</v>
+      </c>
+      <c r="F92" s="106"/>
       <c r="G92" s="13" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="H92" s="13" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="I92" s="6"/>
       <c r="J92" s="6"/>
@@ -12615,26 +12663,26 @@
     </row>
     <row r="93">
       <c r="A93" s="69" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="B93" s="55" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="C93" s="77" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="D93" s="77" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="E93" s="77" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="F93" s="77"/>
       <c r="G93" s="13" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="H93" s="13" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="I93" s="6"/>
       <c r="J93" s="6"/>
@@ -12642,22 +12690,22 @@
     </row>
     <row r="94">
       <c r="A94" s="69" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="B94" s="55" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="C94" s="49"/>
       <c r="D94" s="49"/>
       <c r="E94" s="49" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="F94" s="49"/>
       <c r="G94" s="4" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="H94" s="39" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="I94" s="6"/>
       <c r="J94" s="6"/>
@@ -12665,22 +12713,22 @@
     </row>
     <row r="95">
       <c r="A95" s="69" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B95" s="55" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="C95" s="49"/>
       <c r="D95" s="49"/>
       <c r="E95" s="49" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="F95" s="49"/>
       <c r="G95" s="4" t="s">
-        <v>475</v>
-      </c>
-      <c r="H95" s="95" t="s">
-        <v>480</v>
+        <v>477</v>
+      </c>
+      <c r="H95" s="96" t="s">
+        <v>482</v>
       </c>
       <c r="I95" s="6"/>
       <c r="J95" s="6"/>
@@ -12688,22 +12736,22 @@
     </row>
     <row r="96">
       <c r="A96" s="69" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="B96" s="55" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="C96" s="49"/>
       <c r="D96" s="49"/>
       <c r="E96" s="49" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="F96" s="49"/>
       <c r="G96" s="4" t="s">
-        <v>475</v>
-      </c>
-      <c r="H96" s="95" t="s">
-        <v>484</v>
+        <v>477</v>
+      </c>
+      <c r="H96" s="96" t="s">
+        <v>486</v>
       </c>
       <c r="I96" s="6"/>
       <c r="J96" s="6"/>
@@ -12711,22 +12759,22 @@
     </row>
     <row r="97">
       <c r="A97" s="69" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="B97" s="55" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="C97" s="49"/>
       <c r="D97" s="49"/>
       <c r="E97" s="49" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="F97" s="49"/>
       <c r="G97" s="4" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="H97" s="4" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="I97" s="6"/>
       <c r="J97" s="6"/>
@@ -12734,24 +12782,24 @@
     </row>
     <row r="98">
       <c r="A98" s="69" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="B98" s="55" t="s">
-        <v>490</v>
-      </c>
-      <c r="C98" s="107" t="s">
-        <v>491</v>
+        <v>492</v>
+      </c>
+      <c r="C98" s="108" t="s">
+        <v>493</v>
       </c>
       <c r="D98" s="49"/>
       <c r="E98" s="49" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="F98" s="39"/>
       <c r="G98" s="36" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="H98" s="49" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="I98" s="6"/>
       <c r="J98" s="6"/>
@@ -12759,13 +12807,13 @@
     </row>
     <row r="99">
       <c r="A99" s="48" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="B99" s="47" t="s">
-        <v>496</v>
-      </c>
-      <c r="C99" s="97" t="s">
-        <v>428</v>
+        <v>498</v>
+      </c>
+      <c r="C99" s="98" t="s">
+        <v>430</v>
       </c>
       <c r="D99" s="49"/>
       <c r="E99" s="39"/>
@@ -12778,7 +12826,7 @@
     </row>
     <row r="100">
       <c r="A100" s="69" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="B100" s="55" t="s">
         <v>55</v>
@@ -12790,14 +12838,14 @@
         <v>57</v>
       </c>
       <c r="E100" s="49" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="F100" s="49"/>
       <c r="G100" s="43" t="s">
         <v>59</v>
       </c>
       <c r="H100" s="43" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="I100" s="6"/>
       <c r="J100" s="6"/>
@@ -12805,7 +12853,7 @@
     </row>
     <row r="101">
       <c r="A101" s="69" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="B101" s="55" t="s">
         <v>62</v>
@@ -12817,14 +12865,14 @@
         <v>64</v>
       </c>
       <c r="E101" s="49" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="F101" s="49"/>
       <c r="G101" s="45" t="s">
         <v>66</v>
       </c>
       <c r="H101" s="45" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="I101" s="6"/>
       <c r="J101" s="6"/>
@@ -12832,7 +12880,7 @@
     </row>
     <row r="102">
       <c r="A102" s="69" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="B102" s="55" t="s">
         <v>69</v>
@@ -12844,14 +12892,14 @@
         <v>71</v>
       </c>
       <c r="E102" s="49" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="F102" s="49"/>
       <c r="G102" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="H102" s="95" t="s">
-        <v>505</v>
+      <c r="H102" s="96" t="s">
+        <v>507</v>
       </c>
       <c r="I102" s="6"/>
       <c r="J102" s="6"/>
@@ -12859,7 +12907,7 @@
     </row>
     <row r="103">
       <c r="A103" s="69" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="B103" s="55" t="s">
         <v>76</v>
@@ -12871,14 +12919,14 @@
         <v>78</v>
       </c>
       <c r="E103" s="49" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="F103" s="49"/>
       <c r="G103" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="H103" s="95" t="s">
-        <v>508</v>
+      <c r="H103" s="96" t="s">
+        <v>510</v>
       </c>
       <c r="I103" s="6"/>
       <c r="J103" s="6"/>
@@ -12886,7 +12934,7 @@
     </row>
     <row r="104">
       <c r="A104" s="69" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="B104" s="55" t="s">
         <v>82</v>
@@ -12898,16 +12946,16 @@
         <v>84</v>
       </c>
       <c r="E104" s="39" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="F104" s="39" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="G104" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="H104" s="99" t="s">
-        <v>512</v>
+      <c r="H104" s="100" t="s">
+        <v>514</v>
       </c>
       <c r="I104" s="6"/>
       <c r="J104" s="6"/>
@@ -12915,7 +12963,7 @@
     </row>
     <row r="105">
       <c r="A105" s="69" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="B105" s="55" t="s">
         <v>90</v>
@@ -12924,17 +12972,17 @@
         <v>91</v>
       </c>
       <c r="D105" s="49" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="E105" s="49" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="F105" s="49"/>
       <c r="G105" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="H105" s="95" t="s">
-        <v>516</v>
+      <c r="H105" s="96" t="s">
+        <v>518</v>
       </c>
       <c r="I105" s="6"/>
       <c r="J105" s="6"/>
@@ -12942,7 +12990,7 @@
     </row>
     <row r="106">
       <c r="A106" s="69" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="B106" s="55" t="s">
         <v>97</v>
@@ -12954,14 +13002,14 @@
         <v>99</v>
       </c>
       <c r="E106" s="77" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="F106" s="77"/>
-      <c r="G106" s="108" t="s">
+      <c r="G106" s="109" t="s">
         <v>101</v>
       </c>
-      <c r="H106" s="109" t="s">
-        <v>519</v>
+      <c r="H106" s="110" t="s">
+        <v>521</v>
       </c>
       <c r="I106" s="6"/>
       <c r="J106" s="6"/>
@@ -12969,7 +13017,7 @@
     </row>
     <row r="107">
       <c r="A107" s="69" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="B107" s="55" t="s">
         <v>117</v>
@@ -12981,14 +13029,14 @@
         <v>119</v>
       </c>
       <c r="E107" s="49" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="F107" s="49"/>
       <c r="G107" s="49" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="H107" s="49" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="I107" s="6"/>
       <c r="J107" s="6"/>
@@ -12996,7 +13044,7 @@
     </row>
     <row r="108">
       <c r="A108" s="69" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="B108" s="55" t="s">
         <v>111</v>
@@ -13008,14 +13056,14 @@
         <v>113</v>
       </c>
       <c r="E108" s="49" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="F108" s="49"/>
       <c r="G108" s="49" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="H108" s="49" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="I108" s="6"/>
       <c r="J108" s="6"/>
@@ -13023,10 +13071,10 @@
     </row>
     <row r="109">
       <c r="A109" s="69" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="B109" s="55" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="C109" s="49" t="s">
         <v>133</v>
@@ -13035,14 +13083,14 @@
         <v>134</v>
       </c>
       <c r="E109" s="77" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="F109" s="77"/>
-      <c r="G109" s="110" t="s">
-        <v>522</v>
-      </c>
-      <c r="H109" s="111" t="s">
-        <v>531</v>
+      <c r="G109" s="111" t="s">
+        <v>524</v>
+      </c>
+      <c r="H109" s="112" t="s">
+        <v>533</v>
       </c>
       <c r="I109" s="6"/>
       <c r="J109" s="6"/>
@@ -13050,7 +13098,7 @@
     </row>
     <row r="110">
       <c r="A110" s="69" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="B110" s="55" t="s">
         <v>124</v>
@@ -13062,14 +13110,14 @@
         <v>126</v>
       </c>
       <c r="E110" s="49" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="F110" s="49"/>
       <c r="G110" s="49" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="H110" s="49" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="I110" s="6"/>
       <c r="J110" s="6"/>
@@ -13077,26 +13125,26 @@
     </row>
     <row r="111">
       <c r="A111" s="69" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="B111" s="55" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="C111" s="36" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="D111" s="49" t="s">
-        <v>538</v>
-      </c>
-      <c r="E111" s="112" t="s">
-        <v>539</v>
-      </c>
-      <c r="F111" s="113"/>
+        <v>540</v>
+      </c>
+      <c r="E111" s="113" t="s">
+        <v>541</v>
+      </c>
+      <c r="F111" s="114"/>
       <c r="G111" s="4" t="s">
-        <v>540</v>
-      </c>
-      <c r="H111" s="114" t="s">
-        <v>541</v>
+        <v>542</v>
+      </c>
+      <c r="H111" s="115" t="s">
+        <v>543</v>
       </c>
       <c r="I111" s="6"/>
       <c r="J111" s="6"/>
@@ -13107,15 +13155,15 @@
       <c r="B112" s="4"/>
       <c r="C112" s="77"/>
       <c r="D112" s="77"/>
-      <c r="E112" s="106" t="s">
-        <v>539</v>
+      <c r="E112" s="107" t="s">
+        <v>541</v>
       </c>
       <c r="F112" s="81"/>
-      <c r="G112" s="108" t="s">
-        <v>542</v>
-      </c>
-      <c r="H112" s="108" t="s">
-        <v>543</v>
+      <c r="G112" s="109" t="s">
+        <v>544</v>
+      </c>
+      <c r="H112" s="109" t="s">
+        <v>545</v>
       </c>
       <c r="I112" s="6"/>
       <c r="J112" s="6"/>
@@ -13123,13 +13171,13 @@
     </row>
     <row r="113">
       <c r="A113" s="48" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="B113" s="47" t="s">
-        <v>545</v>
-      </c>
-      <c r="C113" s="103" t="s">
-        <v>428</v>
+        <v>547</v>
+      </c>
+      <c r="C113" s="104" t="s">
+        <v>430</v>
       </c>
       <c r="D113" s="4"/>
       <c r="E113" s="4"/>
@@ -13142,26 +13190,26 @@
     </row>
     <row r="114">
       <c r="A114" s="69" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="B114" s="55" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="C114" s="49" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="D114" s="49" t="s">
         <v>220</v>
       </c>
       <c r="E114" s="49" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="F114" s="49"/>
       <c r="G114" s="36" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="H114" s="49" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="I114" s="6"/>
       <c r="J114" s="6"/>
@@ -13169,24 +13217,24 @@
     </row>
     <row r="115">
       <c r="A115" s="78" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="B115" s="79" t="s">
         <v>225</v>
       </c>
-      <c r="C115" s="115" t="s">
-        <v>553</v>
+      <c r="C115" s="116" t="s">
+        <v>555</v>
       </c>
       <c r="D115" s="49"/>
       <c r="E115" s="49" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="F115" s="49"/>
       <c r="G115" s="36" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="H115" s="49" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="I115" s="6"/>
       <c r="J115" s="6"/>
@@ -13194,26 +13242,26 @@
     </row>
     <row r="116">
       <c r="A116" s="69" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="B116" s="55" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="C116" s="77" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="D116" s="77" t="s">
-        <v>560</v>
-      </c>
-      <c r="E116" s="116" t="s">
-        <v>561</v>
-      </c>
-      <c r="F116" s="116"/>
+        <v>562</v>
+      </c>
+      <c r="E116" s="117" t="s">
+        <v>563</v>
+      </c>
+      <c r="F116" s="117"/>
       <c r="G116" s="4" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="H116" s="81" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="I116" s="6"/>
       <c r="J116" s="6"/>
@@ -13221,24 +13269,24 @@
     </row>
     <row r="117">
       <c r="A117" s="78" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="B117" s="79" t="s">
         <v>225</v>
       </c>
-      <c r="C117" s="115" t="s">
-        <v>553</v>
+      <c r="C117" s="116" t="s">
+        <v>555</v>
       </c>
       <c r="D117" s="49"/>
-      <c r="E117" s="116" t="s">
-        <v>565</v>
-      </c>
-      <c r="F117" s="116"/>
+      <c r="E117" s="117" t="s">
+        <v>567</v>
+      </c>
+      <c r="F117" s="117"/>
       <c r="G117" s="4" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="H117" s="39" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="I117" s="6"/>
       <c r="J117" s="6"/>
@@ -13246,26 +13294,26 @@
     </row>
     <row r="118">
       <c r="A118" s="69" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="B118" s="55" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="C118" s="56" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="D118" s="70" t="s">
-        <v>571</v>
-      </c>
-      <c r="E118" s="117" t="s">
-        <v>572</v>
-      </c>
-      <c r="F118" s="117"/>
+        <v>573</v>
+      </c>
+      <c r="E118" s="118" t="s">
+        <v>574</v>
+      </c>
+      <c r="F118" s="118"/>
       <c r="G118" s="70" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="H118" s="70" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="I118" s="6"/>
       <c r="J118" s="6"/>
@@ -13273,24 +13321,24 @@
     </row>
     <row r="119">
       <c r="A119" s="78" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="B119" s="79" t="s">
         <v>225</v>
       </c>
-      <c r="C119" s="118" t="s">
-        <v>553</v>
+      <c r="C119" s="119" t="s">
+        <v>555</v>
       </c>
       <c r="D119" s="56"/>
-      <c r="E119" s="117" t="s">
-        <v>576</v>
+      <c r="E119" s="118" t="s">
+        <v>578</v>
       </c>
       <c r="F119" s="56"/>
       <c r="G119" s="57" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c r="H119" s="57" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="I119" s="6"/>
       <c r="J119" s="6"/>
@@ -13298,26 +13346,26 @@
     </row>
     <row r="120">
       <c r="A120" s="69" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="B120" s="55" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="C120" s="70" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="D120" s="70" t="s">
-        <v>582</v>
-      </c>
-      <c r="E120" s="119" t="s">
-        <v>583</v>
-      </c>
-      <c r="F120" s="119"/>
+        <v>584</v>
+      </c>
+      <c r="E120" s="120" t="s">
+        <v>585</v>
+      </c>
+      <c r="F120" s="120"/>
       <c r="G120" s="56" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="H120" s="56" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="I120" s="6"/>
       <c r="J120" s="6"/>
@@ -13325,24 +13373,24 @@
     </row>
     <row r="121">
       <c r="A121" s="78" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="B121" s="79" t="s">
         <v>225</v>
       </c>
-      <c r="C121" s="120" t="s">
-        <v>553</v>
+      <c r="C121" s="121" t="s">
+        <v>555</v>
       </c>
       <c r="D121" s="70"/>
-      <c r="E121" s="119" t="s">
-        <v>586</v>
+      <c r="E121" s="120" t="s">
+        <v>588</v>
       </c>
       <c r="F121" s="56"/>
       <c r="G121" s="57" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c r="H121" s="57" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="I121" s="6"/>
       <c r="J121" s="6"/>
@@ -13350,26 +13398,26 @@
     </row>
     <row r="122">
       <c r="A122" s="69" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="B122" s="55" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="C122" s="70" t="s">
         <v>231</v>
       </c>
       <c r="D122" s="70" t="s">
-        <v>590</v>
-      </c>
-      <c r="E122" s="119" t="s">
-        <v>591</v>
-      </c>
-      <c r="F122" s="119"/>
+        <v>592</v>
+      </c>
+      <c r="E122" s="120" t="s">
+        <v>593</v>
+      </c>
+      <c r="F122" s="120"/>
       <c r="G122" s="56" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="H122" s="56" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="I122" s="6"/>
       <c r="J122" s="6"/>
@@ -13377,13 +13425,13 @@
     </row>
     <row r="123">
       <c r="A123" s="89" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="B123" s="34" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c r="C123" s="6"/>
-      <c r="D123" s="6"/>
+      <c r="D123" s="81"/>
       <c r="E123" s="18"/>
       <c r="F123" s="18"/>
       <c r="G123" s="4"/>
@@ -13394,7 +13442,7 @@
     </row>
     <row r="124">
       <c r="A124" s="90" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="B124" s="38" t="s">
         <v>366</v>
@@ -13405,15 +13453,15 @@
       <c r="D124" s="6" t="s">
         <v>368</v>
       </c>
-      <c r="E124" s="116" t="s">
-        <v>597</v>
-      </c>
-      <c r="F124" s="116"/>
-      <c r="G124" s="121" t="s">
+      <c r="E124" s="117" t="s">
+        <v>599</v>
+      </c>
+      <c r="F124" s="117"/>
+      <c r="G124" s="122" t="s">
         <v>180</v>
       </c>
-      <c r="H124" s="122" t="s">
-        <v>598</v>
+      <c r="H124" s="123" t="s">
+        <v>600</v>
       </c>
       <c r="I124" s="6"/>
       <c r="J124" s="6"/>
@@ -13421,17 +13469,17 @@
     </row>
     <row r="125">
       <c r="A125" s="90" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="B125" s="38" t="s">
-        <v>600</v>
-      </c>
-      <c r="C125" s="123" t="s">
-        <v>428</v>
-      </c>
-      <c r="D125" s="6"/>
-      <c r="E125" s="124"/>
-      <c r="F125" s="124"/>
+        <v>602</v>
+      </c>
+      <c r="C125" s="124" t="s">
+        <v>430</v>
+      </c>
+      <c r="D125" s="81"/>
+      <c r="E125" s="125"/>
+      <c r="F125" s="125"/>
       <c r="G125" s="4"/>
       <c r="H125" s="4"/>
       <c r="I125" s="6"/>
@@ -13440,24 +13488,24 @@
     </row>
     <row r="126">
       <c r="A126" s="48" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="B126" s="47" t="s">
-        <v>602</v>
-      </c>
-      <c r="C126" s="125" t="s">
-        <v>428</v>
-      </c>
-      <c r="D126" s="6"/>
-      <c r="E126" s="113" t="s">
-        <v>603</v>
-      </c>
-      <c r="F126" s="116"/>
+        <v>604</v>
+      </c>
+      <c r="C126" s="126" t="s">
+        <v>430</v>
+      </c>
+      <c r="D126" s="81"/>
+      <c r="E126" s="114" t="s">
+        <v>605</v>
+      </c>
+      <c r="F126" s="117"/>
       <c r="G126" s="13" t="s">
         <v>52</v>
       </c>
       <c r="H126" s="13" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="I126" s="6"/>
       <c r="J126" s="6"/>
@@ -13465,7 +13513,7 @@
     </row>
     <row r="127">
       <c r="A127" s="69" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="B127" s="55" t="s">
         <v>55</v>
@@ -13476,15 +13524,15 @@
       <c r="D127" s="77" t="s">
         <v>57</v>
       </c>
-      <c r="E127" s="116" t="s">
-        <v>606</v>
-      </c>
-      <c r="F127" s="116"/>
+      <c r="E127" s="117" t="s">
+        <v>608</v>
+      </c>
+      <c r="F127" s="117"/>
       <c r="G127" s="39" t="s">
         <v>59</v>
       </c>
       <c r="H127" s="39" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="I127" s="6"/>
       <c r="J127" s="6"/>
@@ -13492,7 +13540,7 @@
     </row>
     <row r="128">
       <c r="A128" s="69" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="B128" s="55" t="s">
         <v>69</v>
@@ -13504,14 +13552,14 @@
         <v>71</v>
       </c>
       <c r="E128" s="49" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="F128" s="49"/>
       <c r="G128" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="H128" s="95" t="s">
-        <v>610</v>
+      <c r="H128" s="96" t="s">
+        <v>612</v>
       </c>
       <c r="I128" s="6"/>
       <c r="J128" s="6"/>
@@ -13519,7 +13567,7 @@
     </row>
     <row r="129">
       <c r="A129" s="69" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="B129" s="55" t="s">
         <v>76</v>
@@ -13531,14 +13579,14 @@
         <v>78</v>
       </c>
       <c r="E129" s="49" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="F129" s="49"/>
       <c r="G129" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="H129" s="95" t="s">
-        <v>613</v>
+      <c r="H129" s="96" t="s">
+        <v>615</v>
       </c>
       <c r="I129" s="6"/>
       <c r="J129" s="6"/>
@@ -13546,7 +13594,7 @@
     </row>
     <row r="130">
       <c r="A130" s="69" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="B130" s="55" t="s">
         <v>90</v>
@@ -13555,17 +13603,17 @@
         <v>91</v>
       </c>
       <c r="D130" s="77" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="E130" s="49" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="F130" s="49"/>
       <c r="G130" s="39" t="s">
-        <v>616</v>
-      </c>
-      <c r="H130" s="95" t="s">
-        <v>617</v>
+        <v>618</v>
+      </c>
+      <c r="H130" s="96" t="s">
+        <v>619</v>
       </c>
       <c r="I130" s="6"/>
       <c r="J130" s="6"/>
@@ -13573,7 +13621,7 @@
     </row>
     <row r="131">
       <c r="A131" s="69" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="B131" s="55" t="s">
         <v>97</v>
@@ -13585,14 +13633,14 @@
         <v>99</v>
       </c>
       <c r="E131" s="77" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="F131" s="77"/>
       <c r="G131" s="77" t="s">
         <v>101</v>
       </c>
       <c r="H131" s="77" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="I131" s="6"/>
       <c r="J131" s="6"/>
@@ -13600,7 +13648,7 @@
     </row>
     <row r="132">
       <c r="A132" s="69" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c r="B132" s="55" t="s">
         <v>117</v>
@@ -13612,14 +13660,14 @@
         <v>119</v>
       </c>
       <c r="E132" s="49" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c r="F132" s="49"/>
       <c r="G132" s="49" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="H132" s="49" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="I132" s="6"/>
       <c r="J132" s="6"/>
@@ -13627,7 +13675,7 @@
     </row>
     <row r="133">
       <c r="A133" s="69" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c r="B133" s="55" t="s">
         <v>111</v>
@@ -13639,14 +13687,14 @@
         <v>113</v>
       </c>
       <c r="E133" s="49" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="F133" s="49"/>
       <c r="G133" s="49" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="H133" s="49" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="I133" s="6"/>
       <c r="J133" s="6"/>
@@ -13654,10 +13702,10 @@
     </row>
     <row r="134">
       <c r="A134" s="69" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="B134" s="55" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="C134" s="77" t="s">
         <v>133</v>
@@ -13666,14 +13714,14 @@
         <v>134</v>
       </c>
       <c r="E134" s="49" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="F134" s="49"/>
       <c r="G134" s="45" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="H134" s="45" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="I134" s="6"/>
       <c r="J134" s="6"/>
@@ -13681,7 +13729,7 @@
     </row>
     <row r="135">
       <c r="A135" s="69" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="B135" s="55" t="s">
         <v>124</v>
@@ -13693,14 +13741,14 @@
         <v>126</v>
       </c>
       <c r="E135" s="49" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c r="F135" s="49"/>
       <c r="G135" s="49" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="H135" s="49" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="I135" s="6"/>
       <c r="J135" s="6"/>
@@ -13708,24 +13756,24 @@
     </row>
     <row r="136">
       <c r="A136" s="48" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="B136" s="47" t="s">
-        <v>631</v>
-      </c>
-      <c r="C136" s="125" t="s">
-        <v>428</v>
-      </c>
-      <c r="D136" s="126"/>
+        <v>633</v>
+      </c>
+      <c r="C136" s="126" t="s">
+        <v>430</v>
+      </c>
+      <c r="D136" s="127"/>
       <c r="E136" s="39" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c r="F136" s="36"/>
       <c r="G136" s="36" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="H136" s="36" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="I136" s="6"/>
       <c r="J136" s="6"/>
@@ -13733,7 +13781,7 @@
     </row>
     <row r="137">
       <c r="A137" s="69" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="B137" s="55" t="s">
         <v>55</v>
@@ -13745,14 +13793,14 @@
         <v>57</v>
       </c>
       <c r="E137" s="49" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c r="F137" s="49"/>
       <c r="G137" s="39" t="s">
         <v>59</v>
       </c>
       <c r="H137" s="39" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="I137" s="6"/>
       <c r="J137" s="6"/>
@@ -13760,7 +13808,7 @@
     </row>
     <row r="138">
       <c r="A138" s="69" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="B138" s="55" t="s">
         <v>69</v>
@@ -13772,14 +13820,14 @@
         <v>71</v>
       </c>
       <c r="E138" s="49" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="F138" s="49"/>
       <c r="G138" s="39" t="s">
         <v>73</v>
       </c>
       <c r="H138" s="39" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="I138" s="6"/>
       <c r="J138" s="6"/>
@@ -13787,7 +13835,7 @@
     </row>
     <row r="139">
       <c r="A139" s="69" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="B139" s="55" t="s">
         <v>76</v>
@@ -13799,14 +13847,14 @@
         <v>78</v>
       </c>
       <c r="E139" s="49" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="F139" s="49"/>
       <c r="G139" s="39" t="s">
         <v>73</v>
       </c>
       <c r="H139" s="39" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="I139" s="6"/>
       <c r="J139" s="6"/>
@@ -13814,7 +13862,7 @@
     </row>
     <row r="140">
       <c r="A140" s="69" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="B140" s="55" t="s">
         <v>90</v>
@@ -13823,17 +13871,17 @@
         <v>91</v>
       </c>
       <c r="D140" s="77" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="E140" s="49" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="F140" s="49"/>
       <c r="G140" s="39" t="s">
         <v>94</v>
       </c>
       <c r="H140" s="39" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="I140" s="6"/>
       <c r="J140" s="6"/>
@@ -13841,7 +13889,7 @@
     </row>
     <row r="141">
       <c r="A141" s="69" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="B141" s="55" t="s">
         <v>97</v>
@@ -13853,14 +13901,14 @@
         <v>99</v>
       </c>
       <c r="E141" s="49" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="F141" s="49"/>
       <c r="G141" s="39" t="s">
         <v>101</v>
       </c>
       <c r="H141" s="39" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="I141" s="6"/>
       <c r="J141" s="6"/>
@@ -13868,7 +13916,7 @@
     </row>
     <row r="142">
       <c r="A142" s="69" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="B142" s="55" t="s">
         <v>117</v>
@@ -13880,14 +13928,14 @@
         <v>119</v>
       </c>
       <c r="E142" s="49" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="F142" s="77"/>
       <c r="G142" s="49" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="H142" s="49" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="I142" s="6"/>
       <c r="J142" s="6"/>
@@ -13895,7 +13943,7 @@
     </row>
     <row r="143">
       <c r="A143" s="69" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="B143" s="55" t="s">
         <v>111</v>
@@ -13907,14 +13955,14 @@
         <v>113</v>
       </c>
       <c r="E143" s="49" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="F143" s="49"/>
       <c r="G143" s="49" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="H143" s="49" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="I143" s="6"/>
       <c r="J143" s="6"/>
@@ -13922,10 +13970,10 @@
     </row>
     <row r="144">
       <c r="A144" s="69" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="B144" s="55" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="C144" s="77" t="s">
         <v>133</v>
@@ -13934,14 +13982,14 @@
         <v>134</v>
       </c>
       <c r="E144" s="49" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="F144" s="49"/>
       <c r="G144" s="45" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="H144" s="45" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c r="I144" s="6"/>
       <c r="J144" s="6"/>
@@ -13949,7 +13997,7 @@
     </row>
     <row r="145">
       <c r="A145" s="69" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
       <c r="B145" s="55" t="s">
         <v>124</v>
@@ -13961,14 +14009,14 @@
         <v>126</v>
       </c>
       <c r="E145" s="49" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="F145" s="49"/>
       <c r="G145" s="49" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="H145" s="49" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="I145" s="6"/>
       <c r="J145" s="6"/>
@@ -13976,26 +14024,26 @@
     </row>
     <row r="146">
       <c r="A146" s="48" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="B146" s="47" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="C146" s="77" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="D146" s="77" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="E146" s="49" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="F146" s="49"/>
-      <c r="G146" s="121" t="s">
-        <v>663</v>
-      </c>
-      <c r="H146" s="122" t="s">
-        <v>664</v>
+      <c r="G146" s="122" t="s">
+        <v>665</v>
+      </c>
+      <c r="H146" s="123" t="s">
+        <v>666</v>
       </c>
       <c r="I146" s="6"/>
       <c r="J146" s="6"/>
@@ -14003,22 +14051,22 @@
     </row>
     <row r="147">
       <c r="A147" s="48" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="B147" s="47" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="C147" s="6"/>
-      <c r="D147" s="6"/>
+      <c r="D147" s="81"/>
       <c r="E147" s="39" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="F147" s="36"/>
       <c r="G147" s="36" t="s">
         <v>52</v>
       </c>
       <c r="H147" s="36" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="I147" s="6"/>
       <c r="J147" s="6"/>
@@ -14026,7 +14074,7 @@
     </row>
     <row r="148">
       <c r="A148" s="69" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c r="B148" s="55" t="s">
         <v>55</v>
@@ -14038,14 +14086,14 @@
         <v>57</v>
       </c>
       <c r="E148" s="49" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="F148" s="49"/>
       <c r="G148" s="39" t="s">
         <v>59</v>
       </c>
       <c r="H148" s="39" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="I148" s="6"/>
       <c r="J148" s="6"/>
@@ -14053,7 +14101,7 @@
     </row>
     <row r="149">
       <c r="A149" s="69" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="B149" s="55" t="s">
         <v>69</v>
@@ -14065,14 +14113,14 @@
         <v>71</v>
       </c>
       <c r="E149" s="49" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="F149" s="49"/>
       <c r="G149" s="39" t="s">
         <v>73</v>
       </c>
       <c r="H149" s="39" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="I149" s="6"/>
       <c r="J149" s="6"/>
@@ -14080,7 +14128,7 @@
     </row>
     <row r="150">
       <c r="A150" s="69" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="B150" s="55" t="s">
         <v>76</v>
@@ -14092,14 +14140,14 @@
         <v>78</v>
       </c>
       <c r="E150" s="49" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c r="F150" s="49"/>
       <c r="G150" s="39" t="s">
         <v>73</v>
       </c>
       <c r="H150" s="39" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="I150" s="6"/>
       <c r="J150" s="6"/>
@@ -14107,7 +14155,7 @@
     </row>
     <row r="151">
       <c r="A151" s="69" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="B151" s="55" t="s">
         <v>90</v>
@@ -14116,17 +14164,17 @@
         <v>91</v>
       </c>
       <c r="D151" s="77" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="E151" s="49" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="F151" s="49"/>
       <c r="G151" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="H151" s="95" t="s">
-        <v>679</v>
+      <c r="H151" s="96" t="s">
+        <v>681</v>
       </c>
       <c r="I151" s="6"/>
       <c r="J151" s="6"/>
@@ -14134,7 +14182,7 @@
     </row>
     <row r="152">
       <c r="A152" s="69" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="B152" s="55" t="s">
         <v>97</v>
@@ -14146,14 +14194,14 @@
         <v>99</v>
       </c>
       <c r="E152" s="49" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="F152" s="49"/>
       <c r="G152" s="49" t="s">
         <v>101</v>
       </c>
       <c r="H152" s="49" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="I152" s="6"/>
       <c r="J152" s="6"/>
@@ -14161,7 +14209,7 @@
     </row>
     <row r="153">
       <c r="A153" s="69" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="B153" s="55" t="s">
         <v>117</v>
@@ -14173,14 +14221,14 @@
         <v>119</v>
       </c>
       <c r="E153" s="49" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="F153" s="49"/>
       <c r="G153" s="49" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="H153" s="49" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="I153" s="6"/>
       <c r="J153" s="6"/>
@@ -14188,7 +14236,7 @@
     </row>
     <row r="154">
       <c r="A154" s="69" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="B154" s="55" t="s">
         <v>111</v>
@@ -14200,14 +14248,14 @@
         <v>113</v>
       </c>
       <c r="E154" s="49" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="F154" s="49"/>
       <c r="G154" s="49" t="s">
-        <v>526</v>
-      </c>
-      <c r="H154" s="99" t="s">
-        <v>527</v>
+        <v>528</v>
+      </c>
+      <c r="H154" s="100" t="s">
+        <v>529</v>
       </c>
       <c r="I154" s="6"/>
       <c r="J154" s="6"/>
@@ -14215,10 +14263,10 @@
     </row>
     <row r="155">
       <c r="A155" s="69" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="B155" s="55" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="C155" s="77" t="s">
         <v>133</v>
@@ -14227,14 +14275,14 @@
         <v>134</v>
       </c>
       <c r="E155" s="49" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="F155" s="49"/>
       <c r="G155" s="45" t="s">
-        <v>522</v>
-      </c>
-      <c r="H155" s="127" t="s">
-        <v>689</v>
+        <v>524</v>
+      </c>
+      <c r="H155" s="128" t="s">
+        <v>691</v>
       </c>
       <c r="I155" s="6"/>
       <c r="J155" s="6"/>
@@ -14242,7 +14290,7 @@
     </row>
     <row r="156">
       <c r="A156" s="69" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="B156" s="55" t="s">
         <v>124</v>
@@ -14254,14 +14302,14 @@
         <v>126</v>
       </c>
       <c r="E156" s="77" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="F156" s="77"/>
       <c r="G156" s="49" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="H156" s="49" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="I156" s="6"/>
       <c r="J156" s="6"/>
@@ -14269,44 +14317,44 @@
     </row>
     <row r="157">
       <c r="A157" s="90" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="B157" s="38" t="s">
-        <v>693</v>
-      </c>
-      <c r="C157" s="128" t="s">
-        <v>694</v>
-      </c>
-      <c r="D157" s="128" t="s">
         <v>695</v>
       </c>
-      <c r="E157" s="129" t="s">
+      <c r="C157" s="129" t="s">
         <v>696</v>
       </c>
-      <c r="F157" s="129"/>
+      <c r="D157" s="129" t="s">
+        <v>697</v>
+      </c>
+      <c r="E157" s="130" t="s">
+        <v>698</v>
+      </c>
+      <c r="F157" s="130"/>
       <c r="G157" s="39" t="s">
-        <v>697</v>
-      </c>
-      <c r="H157" s="130" t="s">
-        <v>698</v>
+        <v>699</v>
+      </c>
+      <c r="H157" s="131" t="s">
+        <v>700</v>
       </c>
       <c r="I157" s="6"/>
       <c r="J157" s="6"/>
       <c r="K157" s="6"/>
     </row>
     <row r="158">
-      <c r="A158" s="119" t="s">
-        <v>699</v>
+      <c r="A158" s="120" t="s">
+        <v>701</v>
       </c>
       <c r="B158" s="56" t="s">
-        <v>700</v>
-      </c>
-      <c r="C158" s="131" t="s">
-        <v>428</v>
+        <v>702</v>
+      </c>
+      <c r="C158" s="132" t="s">
+        <v>430</v>
       </c>
       <c r="D158" s="70"/>
       <c r="E158" s="56" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="F158" s="56"/>
       <c r="G158" s="56"/>
@@ -14316,37 +14364,37 @@
       <c r="K158" s="6"/>
     </row>
     <row r="159">
-      <c r="A159" s="119" t="s">
-        <v>702</v>
+      <c r="A159" s="120" t="s">
+        <v>704</v>
       </c>
       <c r="B159" s="56" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="C159" s="70"/>
       <c r="D159" s="70"/>
       <c r="E159" s="56" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="F159" s="56"/>
       <c r="G159" s="56" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="H159" s="56" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="I159" s="6"/>
       <c r="J159" s="6"/>
       <c r="K159" s="6"/>
     </row>
     <row r="160">
-      <c r="A160" s="119" t="s">
-        <v>707</v>
+      <c r="A160" s="120" t="s">
+        <v>709</v>
       </c>
       <c r="B160" s="56" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="C160" s="70" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="D160" s="70"/>
       <c r="E160" s="56"/>
@@ -14358,106 +14406,106 @@
       <c r="K160" s="6"/>
     </row>
     <row r="161">
-      <c r="A161" s="119" t="s">
-        <v>709</v>
+      <c r="A161" s="120" t="s">
+        <v>711</v>
       </c>
       <c r="B161" s="70" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="C161" s="70"/>
       <c r="D161" s="70"/>
       <c r="E161" s="70" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="F161" s="70"/>
       <c r="G161" s="70" t="s">
-        <v>705</v>
-      </c>
-      <c r="H161" s="132" t="s">
-        <v>712</v>
+        <v>707</v>
+      </c>
+      <c r="H161" s="133" t="s">
+        <v>714</v>
       </c>
       <c r="I161" s="6"/>
       <c r="J161" s="6"/>
       <c r="K161" s="6"/>
     </row>
     <row r="162">
-      <c r="A162" s="119" t="s">
-        <v>713</v>
+      <c r="A162" s="120" t="s">
+        <v>715</v>
       </c>
       <c r="B162" s="70" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="C162" s="70"/>
       <c r="D162" s="70"/>
       <c r="E162" s="70" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="F162" s="70"/>
       <c r="G162" s="70" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="H162" s="70" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="I162" s="6"/>
       <c r="J162" s="6"/>
       <c r="K162" s="6"/>
     </row>
     <row r="163">
-      <c r="A163" s="119" t="s">
-        <v>717</v>
+      <c r="A163" s="120" t="s">
+        <v>719</v>
       </c>
       <c r="B163" s="70" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="C163" s="70"/>
       <c r="D163" s="70"/>
       <c r="E163" s="70" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="F163" s="70"/>
       <c r="G163" s="70" t="s">
-        <v>705</v>
-      </c>
-      <c r="H163" s="133" t="s">
-        <v>720</v>
+        <v>707</v>
+      </c>
+      <c r="H163" s="134" t="s">
+        <v>722</v>
       </c>
       <c r="I163" s="6"/>
       <c r="J163" s="6"/>
       <c r="K163" s="6"/>
     </row>
     <row r="164">
-      <c r="A164" s="119" t="s">
-        <v>721</v>
+      <c r="A164" s="120" t="s">
+        <v>723</v>
       </c>
       <c r="B164" s="70" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="C164" s="70"/>
       <c r="D164" s="70"/>
       <c r="E164" s="70" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="F164" s="70"/>
       <c r="G164" s="70" t="s">
-        <v>705</v>
-      </c>
-      <c r="H164" s="133" t="s">
-        <v>724</v>
+        <v>707</v>
+      </c>
+      <c r="H164" s="134" t="s">
+        <v>726</v>
       </c>
       <c r="I164" s="6"/>
       <c r="J164" s="6"/>
       <c r="K164" s="6"/>
     </row>
     <row r="165">
-      <c r="A165" s="119" t="s">
-        <v>725</v>
+      <c r="A165" s="120" t="s">
+        <v>727</v>
       </c>
       <c r="B165" s="70" t="s">
-        <v>726</v>
-      </c>
-      <c r="C165" s="131" t="s">
-        <v>428</v>
+        <v>728</v>
+      </c>
+      <c r="C165" s="132" t="s">
+        <v>430</v>
       </c>
       <c r="D165" s="70"/>
       <c r="E165" s="70"/>
@@ -14469,39 +14517,39 @@
       <c r="K165" s="6"/>
     </row>
     <row r="166">
-      <c r="A166" s="119" t="s">
-        <v>727</v>
+      <c r="A166" s="120" t="s">
+        <v>729</v>
       </c>
       <c r="B166" s="70" t="s">
-        <v>728</v>
-      </c>
-      <c r="C166" s="134" t="s">
-        <v>444</v>
+        <v>730</v>
+      </c>
+      <c r="C166" s="135" t="s">
+        <v>446</v>
       </c>
       <c r="D166" s="70"/>
       <c r="E166" s="70" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="F166" s="70"/>
       <c r="G166" s="70" t="s">
-        <v>705</v>
-      </c>
-      <c r="H166" s="135" t="s">
-        <v>730</v>
+        <v>707</v>
+      </c>
+      <c r="H166" s="136" t="s">
+        <v>732</v>
       </c>
       <c r="I166" s="6"/>
       <c r="J166" s="6"/>
       <c r="K166" s="6"/>
     </row>
     <row r="167">
-      <c r="A167" s="119" t="s">
-        <v>731</v>
+      <c r="A167" s="120" t="s">
+        <v>733</v>
       </c>
       <c r="B167" s="70" t="s">
-        <v>732</v>
-      </c>
-      <c r="C167" s="131" t="s">
-        <v>428</v>
+        <v>734</v>
+      </c>
+      <c r="C167" s="132" t="s">
+        <v>430</v>
       </c>
       <c r="D167" s="70"/>
       <c r="E167" s="70"/>
@@ -14513,27 +14561,27 @@
       <c r="K167" s="6"/>
     </row>
     <row r="168">
-      <c r="A168" s="119" t="s">
-        <v>733</v>
+      <c r="A168" s="120" t="s">
+        <v>735</v>
       </c>
       <c r="B168" s="70" t="s">
-        <v>734</v>
-      </c>
-      <c r="C168" s="131" t="s">
-        <v>735</v>
+        <v>736</v>
+      </c>
+      <c r="C168" s="132" t="s">
+        <v>737</v>
       </c>
       <c r="D168" s="70" t="s">
-        <v>736</v>
-      </c>
-      <c r="E168" s="136" t="s">
-        <v>737</v>
+        <v>738</v>
+      </c>
+      <c r="E168" s="137" t="s">
+        <v>739</v>
       </c>
       <c r="F168" s="70"/>
       <c r="G168" s="70" t="s">
-        <v>738</v>
-      </c>
-      <c r="H168" s="133" t="s">
-        <v>739</v>
+        <v>740</v>
+      </c>
+      <c r="H168" s="134" t="s">
+        <v>741</v>
       </c>
       <c r="I168" s="6"/>
       <c r="J168" s="6"/>
@@ -14570,33 +14618,34 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink r:id="rId2" ref="H80"/>
-    <hyperlink r:id="rId3" ref="H85"/>
-    <hyperlink r:id="rId4" ref="H86"/>
-    <hyperlink r:id="rId5" ref="H87"/>
-    <hyperlink r:id="rId6" ref="H95"/>
-    <hyperlink r:id="rId7" ref="H96"/>
-    <hyperlink r:id="rId8" ref="H102"/>
-    <hyperlink r:id="rId9" ref="H103"/>
-    <hyperlink r:id="rId10" ref="H104"/>
-    <hyperlink r:id="rId11" ref="H105"/>
-    <hyperlink r:id="rId12" ref="H106"/>
-    <hyperlink r:id="rId13" ref="H109"/>
-    <hyperlink r:id="rId14" ref="H111"/>
-    <hyperlink r:id="rId15" ref="H128"/>
-    <hyperlink r:id="rId16" ref="H129"/>
-    <hyperlink r:id="rId17" ref="H130"/>
-    <hyperlink r:id="rId18" ref="H151"/>
-    <hyperlink r:id="rId19" ref="H154"/>
-    <hyperlink r:id="rId20" ref="H155"/>
-    <hyperlink r:id="rId21" ref="H161"/>
-    <hyperlink r:id="rId22" ref="H163"/>
-    <hyperlink r:id="rId23" ref="H164"/>
-    <hyperlink r:id="rId24" ref="H166"/>
-    <hyperlink r:id="rId25" ref="H168"/>
+    <hyperlink r:id="rId2" ref="H73"/>
+    <hyperlink r:id="rId3" ref="H80"/>
+    <hyperlink r:id="rId4" ref="H85"/>
+    <hyperlink r:id="rId5" ref="H86"/>
+    <hyperlink r:id="rId6" ref="H87"/>
+    <hyperlink r:id="rId7" ref="H95"/>
+    <hyperlink r:id="rId8" ref="H96"/>
+    <hyperlink r:id="rId9" ref="H102"/>
+    <hyperlink r:id="rId10" ref="H103"/>
+    <hyperlink r:id="rId11" ref="H104"/>
+    <hyperlink r:id="rId12" ref="H105"/>
+    <hyperlink r:id="rId13" ref="H106"/>
+    <hyperlink r:id="rId14" ref="H109"/>
+    <hyperlink r:id="rId15" ref="H111"/>
+    <hyperlink r:id="rId16" ref="H128"/>
+    <hyperlink r:id="rId17" ref="H129"/>
+    <hyperlink r:id="rId18" ref="H130"/>
+    <hyperlink r:id="rId19" ref="H151"/>
+    <hyperlink r:id="rId20" ref="H154"/>
+    <hyperlink r:id="rId21" ref="H155"/>
+    <hyperlink r:id="rId22" ref="H161"/>
+    <hyperlink r:id="rId23" ref="H163"/>
+    <hyperlink r:id="rId24" ref="H164"/>
+    <hyperlink r:id="rId25" ref="H166"/>
+    <hyperlink r:id="rId26" ref="H168"/>
   </hyperlinks>
-  <drawing r:id="rId26"/>
-  <legacyDrawing r:id="rId27"/>
+  <drawing r:id="rId27"/>
+  <legacyDrawing r:id="rId28"/>
 </worksheet>
 </file>
 
@@ -14617,177 +14666,177 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="137" t="s">
+      <c r="A1" s="138" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="138" t="s">
+      <c r="B1" s="139" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="138" t="s">
+      <c r="C1" s="139" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="138" t="s">
+      <c r="D1" s="139" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="138" t="s">
+      <c r="E1" s="139" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="138" t="s">
+      <c r="F1" s="139" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="18" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="B2" s="39" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="C2" s="77" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="D2" s="77"/>
       <c r="E2" s="39" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
       <c r="F2" s="39" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="18" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="B3" s="81" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="C3" s="77" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="D3" s="77"/>
       <c r="E3" s="39" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="F3" s="39" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="18" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="B4" s="81" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="C4" s="77" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
       <c r="D4" s="77" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
       <c r="E4" s="39" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c r="F4" s="39" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="21" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="B5" s="81" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="E5" s="39" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="F5" s="39" t="s">
-        <v>753</v>
-      </c>
-      <c r="G5" s="139"/>
-      <c r="H5" s="139"/>
-      <c r="I5" s="139"/>
-      <c r="J5" s="139"/>
-      <c r="K5" s="139"/>
-      <c r="L5" s="139"/>
-      <c r="M5" s="139"/>
-      <c r="N5" s="139"/>
-      <c r="O5" s="139"/>
-      <c r="P5" s="139"/>
-      <c r="Q5" s="139"/>
-      <c r="R5" s="139"/>
-      <c r="S5" s="139"/>
-      <c r="T5" s="139"/>
-      <c r="U5" s="139"/>
-      <c r="V5" s="139"/>
-      <c r="W5" s="139"/>
-      <c r="X5" s="139"/>
-      <c r="Y5" s="139"/>
-      <c r="Z5" s="139"/>
+        <v>755</v>
+      </c>
+      <c r="G5" s="140"/>
+      <c r="H5" s="140"/>
+      <c r="I5" s="140"/>
+      <c r="J5" s="140"/>
+      <c r="K5" s="140"/>
+      <c r="L5" s="140"/>
+      <c r="M5" s="140"/>
+      <c r="N5" s="140"/>
+      <c r="O5" s="140"/>
+      <c r="P5" s="140"/>
+      <c r="Q5" s="140"/>
+      <c r="R5" s="140"/>
+      <c r="S5" s="140"/>
+      <c r="T5" s="140"/>
+      <c r="U5" s="140"/>
+      <c r="V5" s="140"/>
+      <c r="W5" s="140"/>
+      <c r="X5" s="140"/>
+      <c r="Y5" s="140"/>
+      <c r="Z5" s="140"/>
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="B6" s="81" t="s">
-        <v>490</v>
-      </c>
-      <c r="C6" s="140" t="s">
-        <v>491</v>
+        <v>492</v>
+      </c>
+      <c r="C6" s="141" t="s">
+        <v>493</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="39" t="s">
-        <v>754</v>
+        <v>756</v>
       </c>
       <c r="F6" s="39" t="s">
-        <v>755</v>
-      </c>
-      <c r="G6" s="139"/>
-      <c r="H6" s="139"/>
-      <c r="I6" s="139"/>
-      <c r="J6" s="139"/>
-      <c r="K6" s="139"/>
-      <c r="L6" s="139"/>
-      <c r="M6" s="139"/>
-      <c r="N6" s="139"/>
-      <c r="O6" s="139"/>
-      <c r="P6" s="139"/>
-      <c r="Q6" s="139"/>
-      <c r="R6" s="139"/>
-      <c r="S6" s="139"/>
-      <c r="T6" s="139"/>
-      <c r="U6" s="139"/>
-      <c r="V6" s="139"/>
-      <c r="W6" s="139"/>
-      <c r="X6" s="139"/>
-      <c r="Y6" s="139"/>
-      <c r="Z6" s="139"/>
+        <v>757</v>
+      </c>
+      <c r="G6" s="140"/>
+      <c r="H6" s="140"/>
+      <c r="I6" s="140"/>
+      <c r="J6" s="140"/>
+      <c r="K6" s="140"/>
+      <c r="L6" s="140"/>
+      <c r="M6" s="140"/>
+      <c r="N6" s="140"/>
+      <c r="O6" s="140"/>
+      <c r="P6" s="140"/>
+      <c r="Q6" s="140"/>
+      <c r="R6" s="140"/>
+      <c r="S6" s="140"/>
+      <c r="T6" s="140"/>
+      <c r="U6" s="140"/>
+      <c r="V6" s="140"/>
+      <c r="W6" s="140"/>
+      <c r="X6" s="140"/>
+      <c r="Y6" s="140"/>
+      <c r="Z6" s="140"/>
     </row>
     <row r="7">
       <c r="A7" s="18" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="B7" s="39" t="s">
-        <v>756</v>
+        <v>758</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="E7" s="39" t="s">
-        <v>757</v>
+        <v>759</v>
       </c>
       <c r="F7" s="39" t="s">
-        <v>758</v>
+        <v>760</v>
       </c>
     </row>
     <row r="8">
@@ -18791,108 +18840,108 @@
   </cols>
   <sheetData>
     <row r="2">
-      <c r="A2" s="141" t="s">
-        <v>759</v>
-      </c>
-      <c r="B2" s="142" t="s">
-        <v>760</v>
+      <c r="A2" s="142" t="s">
+        <v>761</v>
+      </c>
+      <c r="B2" s="143" t="s">
+        <v>762</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="143" t="s">
-        <v>761</v>
-      </c>
-      <c r="B3" s="142" t="s">
-        <v>762</v>
+      <c r="A3" s="144" t="s">
+        <v>763</v>
+      </c>
+      <c r="B3" s="143" t="s">
+        <v>764</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="144" t="s">
-        <v>763</v>
+      <c r="A4" s="145" t="s">
+        <v>765</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="145" t="s">
-        <v>764</v>
-      </c>
-      <c r="B6" s="142" t="s">
-        <v>765</v>
+      <c r="A6" s="146" t="s">
+        <v>766</v>
+      </c>
+      <c r="B6" s="143" t="s">
+        <v>767</v>
       </c>
     </row>
     <row r="7">
-      <c r="B7" s="142" t="s">
-        <v>766</v>
+      <c r="B7" s="143" t="s">
+        <v>768</v>
       </c>
     </row>
     <row r="8">
-      <c r="B8" s="142"/>
+      <c r="B8" s="143"/>
     </row>
     <row r="9">
-      <c r="B9" s="142"/>
+      <c r="B9" s="143"/>
     </row>
     <row r="10">
-      <c r="A10" s="145" t="s">
-        <v>767</v>
+      <c r="A10" s="146" t="s">
+        <v>769</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="145" t="s">
-        <v>768</v>
-      </c>
-      <c r="B11" s="146" t="s">
-        <v>769</v>
+      <c r="A11" s="146" t="s">
+        <v>770</v>
+      </c>
+      <c r="B11" s="147" t="s">
+        <v>771</v>
       </c>
     </row>
     <row r="12">
-      <c r="B12" s="147" t="s">
-        <v>770</v>
+      <c r="B12" s="148" t="s">
+        <v>772</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="148"/>
-      <c r="B13" s="149" t="s">
-        <v>771</v>
+      <c r="A13" s="149"/>
+      <c r="B13" s="150" t="s">
+        <v>773</v>
       </c>
     </row>
     <row r="14">
-      <c r="B14" s="150" t="s">
-        <v>772</v>
+      <c r="B14" s="151" t="s">
+        <v>774</v>
       </c>
     </row>
     <row r="15">
-      <c r="B15" s="151" t="s">
-        <v>773</v>
+      <c r="B15" s="152" t="s">
+        <v>775</v>
       </c>
     </row>
     <row r="16">
-      <c r="B16" s="152" t="s">
-        <v>774</v>
+      <c r="B16" s="153" t="s">
+        <v>776</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="145"/>
+      <c r="A17" s="146"/>
       <c r="B17" s="28"/>
     </row>
     <row r="18">
-      <c r="A18" s="145" t="s">
-        <v>775</v>
-      </c>
-      <c r="B18" s="153" t="s">
-        <v>776</v>
+      <c r="A18" s="146" t="s">
+        <v>777</v>
+      </c>
+      <c r="B18" s="154" t="s">
+        <v>778</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>777</v>
-      </c>
-      <c r="B19" s="154"/>
+        <v>779</v>
+      </c>
+      <c r="B19" s="155"/>
     </row>
     <row r="21">
-      <c r="A21" s="145" t="s">
-        <v>778</v>
-      </c>
-      <c r="B21" s="155" t="s">
-        <v>779</v>
+      <c r="A21" s="146" t="s">
+        <v>780</v>
+      </c>
+      <c r="B21" s="156" t="s">
+        <v>781</v>
       </c>
     </row>
   </sheetData>
@@ -18918,62 +18967,62 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="36" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="36" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>786</v>
+        <v>788</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="36" t="s">
-        <v>787</v>
+        <v>789</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>788</v>
+        <v>790</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
-        <v>790</v>
+        <v>792</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
     </row>
   </sheetData>
@@ -18999,59 +19048,59 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>780</v>
-      </c>
-      <c r="B1" s="156" t="s">
-        <v>792</v>
+        <v>782</v>
+      </c>
+      <c r="B1" s="157" t="s">
+        <v>794</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="157" t="s">
-        <v>793</v>
+      <c r="A2" s="158" t="s">
+        <v>795</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>794</v>
+        <v>796</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="157" t="s">
-        <v>795</v>
+      <c r="A3" s="158" t="s">
+        <v>797</v>
       </c>
       <c r="B3" s="6"/>
     </row>
     <row r="4">
-      <c r="A4" s="157" t="s">
-        <v>796</v>
+      <c r="A4" s="158" t="s">
+        <v>798</v>
       </c>
       <c r="B4" s="6"/>
     </row>
     <row r="5">
-      <c r="A5" s="157" t="s">
-        <v>797</v>
+      <c r="A5" s="158" t="s">
+        <v>799</v>
       </c>
       <c r="B5" s="6"/>
     </row>
     <row r="6">
-      <c r="A6" s="157" t="s">
-        <v>798</v>
+      <c r="A6" s="158" t="s">
+        <v>800</v>
       </c>
       <c r="B6" s="6"/>
     </row>
     <row r="7">
-      <c r="A7" s="157" t="s">
-        <v>799</v>
+      <c r="A7" s="158" t="s">
+        <v>801</v>
       </c>
       <c r="B7" s="6"/>
     </row>
     <row r="8">
-      <c r="A8" s="157" t="s">
-        <v>800</v>
+      <c r="A8" s="158" t="s">
+        <v>802</v>
       </c>
       <c r="B8" s="6"/>
     </row>
     <row r="9">
-      <c r="A9" s="158" t="s">
-        <v>801</v>
+      <c r="A9" s="159" t="s">
+        <v>803</v>
       </c>
       <c r="B9" s="6"/>
     </row>
@@ -19071,7 +19120,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="146"/>
+      <c r="A1" s="147"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -19095,36 +19144,36 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="159" t="s">
-        <v>802</v>
-      </c>
-      <c r="C1" s="159" t="s">
-        <v>803</v>
+      <c r="A1" s="160" t="s">
+        <v>804</v>
+      </c>
+      <c r="C1" s="160" t="s">
+        <v>805</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="145" t="s">
-        <v>804</v>
-      </c>
-      <c r="B2" s="145" t="s">
-        <v>805</v>
-      </c>
-      <c r="C2" s="145" t="s">
+      <c r="A2" s="146" t="s">
         <v>806</v>
       </c>
-      <c r="D2" s="145" t="s">
+      <c r="B2" s="146" t="s">
         <v>807</v>
+      </c>
+      <c r="C2" s="146" t="s">
+        <v>808</v>
+      </c>
+      <c r="D2" s="146" t="s">
+        <v>809</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="39" t="s">
-        <v>808</v>
+        <v>810</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>809</v>
+        <v>811</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="D3" s="4" t="str">
         <f t="shared" ref="D3:D4" si="1">RIGHT(A3,LEN(A3) - (FIND(" == ",A3) + 3))</f>
@@ -19155,13 +19204,13 @@
     </row>
     <row r="4">
       <c r="A4" s="39" t="s">
+        <v>813</v>
+      </c>
+      <c r="B4" s="39" t="s">
         <v>811</v>
       </c>
-      <c r="B4" s="39" t="s">
-        <v>809</v>
-      </c>
       <c r="C4" s="4" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="D4" s="4" t="str">
         <f t="shared" si="1"/>
@@ -19192,13 +19241,13 @@
     </row>
     <row r="5">
       <c r="A5" s="39" t="s">
+        <v>814</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>815</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>812</v>
-      </c>
-      <c r="B5" s="39" t="s">
-        <v>813</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>810</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -19226,16 +19275,16 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>816</v>
+        <v>818</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -19262,16 +19311,16 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>817</v>
+        <v>819</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>818</v>
+        <v>820</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>810</v>
-      </c>
-      <c r="D7" s="160" t="s">
-        <v>819</v>
+        <v>812</v>
+      </c>
+      <c r="D7" s="161" t="s">
+        <v>821</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -19298,16 +19347,16 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>820</v>
+        <v>822</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -19333,220 +19382,220 @@
       <c r="Z8" s="6"/>
     </row>
     <row r="9">
-      <c r="A9" s="161" t="s">
-        <v>823</v>
-      </c>
-      <c r="B9" s="162" t="s">
-        <v>824</v>
-      </c>
-      <c r="C9" s="162" t="s">
-        <v>810</v>
-      </c>
-      <c r="D9" s="162" t="s">
+      <c r="A9" s="162" t="s">
         <v>825</v>
       </c>
-      <c r="E9" s="162"/>
-      <c r="F9" s="162"/>
-      <c r="G9" s="162"/>
-      <c r="H9" s="162"/>
-      <c r="I9" s="162"/>
-      <c r="J9" s="162"/>
-      <c r="K9" s="162"/>
-      <c r="L9" s="162"/>
-      <c r="M9" s="162"/>
-      <c r="N9" s="162"/>
-      <c r="O9" s="162"/>
-      <c r="P9" s="162"/>
-      <c r="Q9" s="162"/>
-      <c r="R9" s="162"/>
-      <c r="S9" s="162"/>
-      <c r="T9" s="162"/>
-      <c r="U9" s="162"/>
-      <c r="V9" s="162"/>
-      <c r="W9" s="162"/>
-      <c r="X9" s="162"/>
-      <c r="Y9" s="162"/>
-      <c r="Z9" s="162"/>
+      <c r="B9" s="163" t="s">
+        <v>826</v>
+      </c>
+      <c r="C9" s="163" t="s">
+        <v>812</v>
+      </c>
+      <c r="D9" s="163" t="s">
+        <v>827</v>
+      </c>
+      <c r="E9" s="163"/>
+      <c r="F9" s="163"/>
+      <c r="G9" s="163"/>
+      <c r="H9" s="163"/>
+      <c r="I9" s="163"/>
+      <c r="J9" s="163"/>
+      <c r="K9" s="163"/>
+      <c r="L9" s="163"/>
+      <c r="M9" s="163"/>
+      <c r="N9" s="163"/>
+      <c r="O9" s="163"/>
+      <c r="P9" s="163"/>
+      <c r="Q9" s="163"/>
+      <c r="R9" s="163"/>
+      <c r="S9" s="163"/>
+      <c r="T9" s="163"/>
+      <c r="U9" s="163"/>
+      <c r="V9" s="163"/>
+      <c r="W9" s="163"/>
+      <c r="X9" s="163"/>
+      <c r="Y9" s="163"/>
+      <c r="Z9" s="163"/>
     </row>
     <row r="10">
-      <c r="A10" s="161" t="s">
+      <c r="A10" s="162" t="s">
+        <v>828</v>
+      </c>
+      <c r="B10" s="163" t="s">
         <v>826</v>
       </c>
-      <c r="B10" s="162" t="s">
-        <v>824</v>
-      </c>
-      <c r="C10" s="162" t="s">
-        <v>810</v>
-      </c>
-      <c r="D10" s="162" t="s">
-        <v>827</v>
-      </c>
-      <c r="E10" s="162"/>
-      <c r="F10" s="162"/>
-      <c r="G10" s="162"/>
-      <c r="H10" s="162"/>
-      <c r="I10" s="162"/>
-      <c r="J10" s="162"/>
-      <c r="K10" s="162"/>
-      <c r="L10" s="162"/>
-      <c r="M10" s="162"/>
-      <c r="N10" s="162"/>
-      <c r="O10" s="162"/>
-      <c r="P10" s="162"/>
-      <c r="Q10" s="162"/>
-      <c r="R10" s="162"/>
-      <c r="S10" s="162"/>
-      <c r="T10" s="162"/>
-      <c r="U10" s="162"/>
-      <c r="V10" s="162"/>
-      <c r="W10" s="162"/>
-      <c r="X10" s="162"/>
-      <c r="Y10" s="162"/>
-      <c r="Z10" s="162"/>
+      <c r="C10" s="163" t="s">
+        <v>812</v>
+      </c>
+      <c r="D10" s="163" t="s">
+        <v>829</v>
+      </c>
+      <c r="E10" s="163"/>
+      <c r="F10" s="163"/>
+      <c r="G10" s="163"/>
+      <c r="H10" s="163"/>
+      <c r="I10" s="163"/>
+      <c r="J10" s="163"/>
+      <c r="K10" s="163"/>
+      <c r="L10" s="163"/>
+      <c r="M10" s="163"/>
+      <c r="N10" s="163"/>
+      <c r="O10" s="163"/>
+      <c r="P10" s="163"/>
+      <c r="Q10" s="163"/>
+      <c r="R10" s="163"/>
+      <c r="S10" s="163"/>
+      <c r="T10" s="163"/>
+      <c r="U10" s="163"/>
+      <c r="V10" s="163"/>
+      <c r="W10" s="163"/>
+      <c r="X10" s="163"/>
+      <c r="Y10" s="163"/>
+      <c r="Z10" s="163"/>
     </row>
     <row r="11">
-      <c r="A11" s="161" t="s">
-        <v>828</v>
-      </c>
-      <c r="B11" s="162" t="s">
-        <v>829</v>
-      </c>
-      <c r="C11" s="162" t="s">
-        <v>810</v>
-      </c>
-      <c r="D11" s="162" t="s">
+      <c r="A11" s="162" t="s">
         <v>830</v>
       </c>
-      <c r="E11" s="162"/>
-      <c r="F11" s="162"/>
-      <c r="G11" s="162"/>
-      <c r="H11" s="162"/>
-      <c r="I11" s="162"/>
-      <c r="J11" s="162"/>
-      <c r="K11" s="162"/>
-      <c r="L11" s="162"/>
-      <c r="M11" s="162"/>
-      <c r="N11" s="162"/>
-      <c r="O11" s="162"/>
-      <c r="P11" s="162"/>
-      <c r="Q11" s="162"/>
-      <c r="R11" s="162"/>
-      <c r="S11" s="162"/>
-      <c r="T11" s="162"/>
-      <c r="U11" s="162"/>
-      <c r="V11" s="162"/>
-      <c r="W11" s="162"/>
-      <c r="X11" s="162"/>
-      <c r="Y11" s="162"/>
-      <c r="Z11" s="162"/>
+      <c r="B11" s="163" t="s">
+        <v>831</v>
+      </c>
+      <c r="C11" s="163" t="s">
+        <v>812</v>
+      </c>
+      <c r="D11" s="163" t="s">
+        <v>832</v>
+      </c>
+      <c r="E11" s="163"/>
+      <c r="F11" s="163"/>
+      <c r="G11" s="163"/>
+      <c r="H11" s="163"/>
+      <c r="I11" s="163"/>
+      <c r="J11" s="163"/>
+      <c r="K11" s="163"/>
+      <c r="L11" s="163"/>
+      <c r="M11" s="163"/>
+      <c r="N11" s="163"/>
+      <c r="O11" s="163"/>
+      <c r="P11" s="163"/>
+      <c r="Q11" s="163"/>
+      <c r="R11" s="163"/>
+      <c r="S11" s="163"/>
+      <c r="T11" s="163"/>
+      <c r="U11" s="163"/>
+      <c r="V11" s="163"/>
+      <c r="W11" s="163"/>
+      <c r="X11" s="163"/>
+      <c r="Y11" s="163"/>
+      <c r="Z11" s="163"/>
     </row>
     <row r="12">
-      <c r="A12" s="161" t="s">
+      <c r="A12" s="162" t="s">
+        <v>833</v>
+      </c>
+      <c r="B12" s="163" t="s">
         <v>831</v>
       </c>
-      <c r="B12" s="162" t="s">
-        <v>829</v>
-      </c>
-      <c r="C12" s="162" t="s">
-        <v>810</v>
-      </c>
-      <c r="D12" s="162" t="s">
-        <v>832</v>
-      </c>
-      <c r="E12" s="162"/>
-      <c r="F12" s="162"/>
-      <c r="G12" s="162"/>
-      <c r="H12" s="162"/>
-      <c r="I12" s="162"/>
-      <c r="J12" s="162"/>
-      <c r="K12" s="162"/>
-      <c r="L12" s="162"/>
-      <c r="M12" s="162"/>
-      <c r="N12" s="162"/>
-      <c r="O12" s="162"/>
-      <c r="P12" s="162"/>
-      <c r="Q12" s="162"/>
-      <c r="R12" s="162"/>
-      <c r="S12" s="162"/>
-      <c r="T12" s="162"/>
-      <c r="U12" s="162"/>
-      <c r="V12" s="162"/>
-      <c r="W12" s="162"/>
-      <c r="X12" s="162"/>
-      <c r="Y12" s="162"/>
-      <c r="Z12" s="162"/>
+      <c r="C12" s="163" t="s">
+        <v>812</v>
+      </c>
+      <c r="D12" s="163" t="s">
+        <v>834</v>
+      </c>
+      <c r="E12" s="163"/>
+      <c r="F12" s="163"/>
+      <c r="G12" s="163"/>
+      <c r="H12" s="163"/>
+      <c r="I12" s="163"/>
+      <c r="J12" s="163"/>
+      <c r="K12" s="163"/>
+      <c r="L12" s="163"/>
+      <c r="M12" s="163"/>
+      <c r="N12" s="163"/>
+      <c r="O12" s="163"/>
+      <c r="P12" s="163"/>
+      <c r="Q12" s="163"/>
+      <c r="R12" s="163"/>
+      <c r="S12" s="163"/>
+      <c r="T12" s="163"/>
+      <c r="U12" s="163"/>
+      <c r="V12" s="163"/>
+      <c r="W12" s="163"/>
+      <c r="X12" s="163"/>
+      <c r="Y12" s="163"/>
+      <c r="Z12" s="163"/>
     </row>
     <row r="13">
-      <c r="A13" s="161" t="s">
-        <v>833</v>
-      </c>
-      <c r="B13" s="161" t="s">
-        <v>813</v>
-      </c>
-      <c r="C13" s="162" t="s">
-        <v>810</v>
-      </c>
-      <c r="D13" s="162" t="s">
-        <v>834</v>
-      </c>
-      <c r="E13" s="162"/>
-      <c r="F13" s="162"/>
-      <c r="G13" s="162"/>
-      <c r="H13" s="162"/>
-      <c r="I13" s="162"/>
-      <c r="J13" s="162"/>
-      <c r="K13" s="162"/>
-      <c r="L13" s="162"/>
-      <c r="M13" s="162"/>
-      <c r="N13" s="162"/>
-      <c r="O13" s="162"/>
-      <c r="P13" s="162"/>
-      <c r="Q13" s="162"/>
-      <c r="R13" s="162"/>
-      <c r="S13" s="162"/>
-      <c r="T13" s="162"/>
-      <c r="U13" s="162"/>
-      <c r="V13" s="162"/>
-      <c r="W13" s="162"/>
-      <c r="X13" s="162"/>
-      <c r="Y13" s="162"/>
-      <c r="Z13" s="162"/>
+      <c r="A13" s="162" t="s">
+        <v>835</v>
+      </c>
+      <c r="B13" s="162" t="s">
+        <v>815</v>
+      </c>
+      <c r="C13" s="163" t="s">
+        <v>812</v>
+      </c>
+      <c r="D13" s="163" t="s">
+        <v>836</v>
+      </c>
+      <c r="E13" s="163"/>
+      <c r="F13" s="163"/>
+      <c r="G13" s="163"/>
+      <c r="H13" s="163"/>
+      <c r="I13" s="163"/>
+      <c r="J13" s="163"/>
+      <c r="K13" s="163"/>
+      <c r="L13" s="163"/>
+      <c r="M13" s="163"/>
+      <c r="N13" s="163"/>
+      <c r="O13" s="163"/>
+      <c r="P13" s="163"/>
+      <c r="Q13" s="163"/>
+      <c r="R13" s="163"/>
+      <c r="S13" s="163"/>
+      <c r="T13" s="163"/>
+      <c r="U13" s="163"/>
+      <c r="V13" s="163"/>
+      <c r="W13" s="163"/>
+      <c r="X13" s="163"/>
+      <c r="Y13" s="163"/>
+      <c r="Z13" s="163"/>
     </row>
     <row r="14">
-      <c r="A14" s="161" t="s">
-        <v>835</v>
-      </c>
-      <c r="B14" s="161" t="s">
-        <v>813</v>
-      </c>
-      <c r="C14" s="162" t="s">
-        <v>810</v>
-      </c>
-      <c r="D14" s="162" t="s">
-        <v>836</v>
-      </c>
-      <c r="E14" s="162"/>
-      <c r="F14" s="162"/>
-      <c r="G14" s="162"/>
-      <c r="H14" s="162"/>
-      <c r="I14" s="162"/>
-      <c r="J14" s="162"/>
-      <c r="K14" s="162"/>
-      <c r="L14" s="162"/>
-      <c r="M14" s="162"/>
-      <c r="N14" s="162"/>
-      <c r="O14" s="162"/>
-      <c r="P14" s="162"/>
-      <c r="Q14" s="162"/>
-      <c r="R14" s="162"/>
-      <c r="S14" s="162"/>
-      <c r="T14" s="162"/>
-      <c r="U14" s="162"/>
-      <c r="V14" s="162"/>
-      <c r="W14" s="162"/>
-      <c r="X14" s="162"/>
-      <c r="Y14" s="162"/>
-      <c r="Z14" s="162"/>
+      <c r="A14" s="162" t="s">
+        <v>837</v>
+      </c>
+      <c r="B14" s="162" t="s">
+        <v>815</v>
+      </c>
+      <c r="C14" s="163" t="s">
+        <v>812</v>
+      </c>
+      <c r="D14" s="163" t="s">
+        <v>838</v>
+      </c>
+      <c r="E14" s="163"/>
+      <c r="F14" s="163"/>
+      <c r="G14" s="163"/>
+      <c r="H14" s="163"/>
+      <c r="I14" s="163"/>
+      <c r="J14" s="163"/>
+      <c r="K14" s="163"/>
+      <c r="L14" s="163"/>
+      <c r="M14" s="163"/>
+      <c r="N14" s="163"/>
+      <c r="O14" s="163"/>
+      <c r="P14" s="163"/>
+      <c r="Q14" s="163"/>
+      <c r="R14" s="163"/>
+      <c r="S14" s="163"/>
+      <c r="T14" s="163"/>
+      <c r="U14" s="163"/>
+      <c r="V14" s="163"/>
+      <c r="W14" s="163"/>
+      <c r="X14" s="163"/>
+      <c r="Y14" s="163"/>
+      <c r="Z14" s="163"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -19574,52 +19623,52 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="159" t="s">
-        <v>802</v>
+      <c r="A1" s="160" t="s">
+        <v>804</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="145" t="s">
-        <v>804</v>
-      </c>
-      <c r="B2" s="145" t="s">
-        <v>805</v>
-      </c>
-      <c r="C2" s="145" t="s">
+      <c r="A2" s="146" t="s">
         <v>806</v>
       </c>
-      <c r="D2" s="145" t="s">
+      <c r="B2" s="146" t="s">
         <v>807</v>
       </c>
+      <c r="C2" s="146" t="s">
+        <v>808</v>
+      </c>
+      <c r="D2" s="146" t="s">
+        <v>809</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="142" t="s">
-        <v>837</v>
-      </c>
-      <c r="B3" s="142" t="s">
-        <v>838</v>
+      <c r="A3" s="143" t="s">
+        <v>839</v>
+      </c>
+      <c r="B3" s="143" t="s">
+        <v>840</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="142" t="s">
-        <v>839</v>
-      </c>
-      <c r="B4" s="142" t="s">
-        <v>840</v>
+      <c r="A4" s="143" t="s">
+        <v>841</v>
+      </c>
+      <c r="B4" s="143" t="s">
+        <v>842</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="142" t="s">
-        <v>841</v>
-      </c>
-      <c r="B5" s="142" t="s">
+      <c r="A5" s="143" t="s">
+        <v>843</v>
+      </c>
+      <c r="B5" s="143" t="s">
+        <v>844</v>
+      </c>
+      <c r="C5" s="164" t="s">
         <v>842</v>
       </c>
-      <c r="C5" s="163" t="s">
-        <v>840</v>
-      </c>
-      <c r="D5" s="142" t="s">
-        <v>843</v>
+      <c r="D5" s="143" t="s">
+        <v>845</v>
       </c>
     </row>
   </sheetData>

</xml_diff>